<commit_message>
Update TC001 for Add To Cart func
</commit_message>
<xml_diff>
--- a/ZombieClothing Manual TCs_VinhTran.xlsx
+++ b/ZombieClothing Manual TCs_VinhTran.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\REFERENCES\VLU-SENIOR.SEMES1\AUTE\Project Manual TCs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E83E338-0C55-4710-AA19-100F875F754E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843894E7-B795-4F33-9ACB-00D8452C8F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" firstSheet="4" activeTab="5" xr2:uid="{D5A25300-DCC6-4734-BB7F-F53EA33C6D7D}"/>
+    <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" firstSheet="4" activeTab="6" xr2:uid="{D5A25300-DCC6-4734-BB7F-F53EA33C6D7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Func- &lt;&lt;Log in&gt;&gt;" sheetId="2" r:id="rId1"/>
     <sheet name="Func- &lt;&lt;Log out&gt;&gt;" sheetId="7" r:id="rId2"/>
     <sheet name="Func- &lt;&lt;Sign up&gt;&gt;" sheetId="3" r:id="rId3"/>
     <sheet name="Func- &lt;&lt;Homepage nav&gt;&gt;" sheetId="4" r:id="rId4"/>
-    <sheet name="Func- &lt;&lt;View new product&gt;&gt;" sheetId="9" r:id="rId5"/>
+    <sheet name="Func- &lt;&lt;View new pro detail&gt;&gt;" sheetId="9" r:id="rId5"/>
     <sheet name="Func- &lt;&lt;Search pro by name&gt;&gt;" sheetId="10" r:id="rId6"/>
     <sheet name="Func- &lt;&lt;Add to cart&gt;&gt;" sheetId="12" r:id="rId7"/>
   </sheets>
@@ -31,7 +31,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Func- &lt;&lt;Log out&gt;&gt;'!$A$22:$L$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Func- &lt;&lt;Search pro by name&gt;&gt;'!$A$22:$L$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Func- &lt;&lt;Sign up&gt;&gt;'!$A$22:$L$22</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Func- &lt;&lt;View new product&gt;&gt;'!$A$22:$L$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Func- &lt;&lt;View new pro detail&gt;&gt;'!$A$22:$L$22</definedName>
     <definedName name="abc">#REF!</definedName>
     <definedName name="Check_inputed_mail_address">#REF!</definedName>
     <definedName name="CS_IT_1.1_001">#REF!</definedName>
@@ -740,7 +740,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="220">
   <si>
     <t>Func - Module</t>
   </si>
@@ -1404,6 +1404,163 @@
   <si>
     <t>Search product by name</t>
   </si>
+  <si>
+    <t>2. Click vào một sản phẩm từ trang chủ</t>
+  </si>
+  <si>
+    <t>3. Click vào nút Thêm vào giỏ hàng</t>
+  </si>
+  <si>
+    <t>4. Click vào nút Xem giỏ hàng được popped up</t>
+  </si>
+  <si>
+    <t>Kiểm tra rằng user add to cart thành công khi thêm 1 sản phẩm vào giỏ hàng với số lượng 1</t>
+  </si>
+  <si>
+    <t>Kiểm tra rằng user add to cart thành công khi thêm 1 sản phẩm vào giỏ hàng với số lượng nhiều hơn 1</t>
+  </si>
+  <si>
+    <t>5. Kiểm tra các thông tin có hợp lệ tại trang Giỏ hàng của bạn</t>
+  </si>
+  <si>
+    <t>1&lt;=${toTalProduct}&lt;=100</t>
+  </si>
+  <si>
+    <t>6. Click vào nút Thêm vào giỏ hàng</t>
+  </si>
+  <si>
+    <t>Kiểm tra rằng user add to cart thành công khi thêm nhiều hơn 1 sản phẩm khác nhau vào giỏ hàng với số lượng 1 cho mỗi sản phẩm</t>
+  </si>
+  <si>
+    <t>7. Nếu muốn thêm nhiều hơn 2 sản phẩm có thể lặp lại step 4, 5, 6</t>
+  </si>
+  <si>
+    <t>5. Click vào một sản phẩm khác từ trang chủ</t>
+  </si>
+  <si>
+    <t>8. Click vào nút Xem giỏ hàng được popped up</t>
+  </si>
+  <si>
+    <t>9. Kiểm tra các thông tin có hợp lệ tại trang Giỏ hàng của bạn</t>
+  </si>
+  <si>
+    <t>1&lt;=${toTalProduct}&lt;=5</t>
+  </si>
+  <si>
+    <t>4. Click vào nút Tiếp tục mua hàng để quay về trang chủ</t>
+  </si>
+  <si>
+    <t>Kiểm tra rằng user xóa sản phẩm khỏi Giỏ hàng thành công sau khi Add to cart</t>
+  </si>
+  <si>
+    <t>5. Xóa hết các sản phẩm có trong Giỏ hàng</t>
+  </si>
+  <si>
+    <r>
+      <t>- Hệ thống navigate user vào trang Giỏ hàng của bạn khi click vào nút Xem giỏ hàng từ pop up theo URL: ""https://zombieclothingstore.com/cart"
+- Hệ thống hiển thị heading page là Giỏ hàng của bạn
+- Hệ thống hiển thị Có ${totalProduct}</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> sản phẩm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> trong giỏ hàng
+- Hệ thống hiển thị tổng tiền bằng tổng giá tri của các sản phẩm được thêm vào
+- Add to cart thành công!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>- Hệ thống navigate user vào trang Giỏ hàng của bạn theo URL: ""https://zombieclothingstore.com/cart"
+- Hệ thống hiển thị heading page là Giỏ hàng của bạn
+- Hệ thống hiển thị Có ${totalProduct}</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> sản phẩm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> trong giỏ hàng
+- Hệ thống hiển thị tổng tiền bằng tổng giá tri của các sản phẩm được thêm vào
+- Add to cart thành công!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Hệ thống navigate user vào trang Giỏ hàng của bạn theo URL: ""https://zombieclothingstore.com/cart"
+- Hệ thống hiển thị heading page là Giỏ hàng của bạn
+- Hệ thống hiển thị Có </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1 sản phẩm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> trong giỏ hàng
+- Hệ thống hiển thị tổng tiền bằng giá tri của sản phẩm được thêm vào
+- Add to cart thành công!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Hệ thống navigate user vào trang Giỏ hàng của bạn theo URL: "https://zombieclothingstore.com/cart"
+- Hệ thống hiển thị Có </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0 sản phẩm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> trong giỏ hàng
+- Hệ thống hiển thị Giỏ hàng của bạn đang trống tại box chứa các sản phẩm được thêm vào
+- Xóa sản phẩm khỏi giỏ hàng thành công!</t>
+    </r>
+  </si>
+  <si>
+    <t>6. Kiểm tra lại các thông tin được hiển thị có hợp lệ khi Xóa sản phẩm khỏi Giỏ hàng</t>
+  </si>
 </sst>
 </file>
 
@@ -1709,7 +1866,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1983,6 +2140,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2838,7 +2998,7 @@
   </sheetPr>
   <dimension ref="A1:AU242"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
@@ -12856,7 +13016,7 @@
   </sheetPr>
   <dimension ref="A1:AU207"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
@@ -13355,7 +13515,7 @@
       <c r="K23" s="33"/>
       <c r="L23" s="33"/>
     </row>
-    <row r="24" spans="1:12" s="28" customFormat="1" ht="55.2" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="24" spans="1:12" s="28" customFormat="1" ht="55.2" customHeight="1" outlineLevel="1">
       <c r="A24" s="49"/>
       <c r="B24" s="52" t="s">
         <v>98</v>
@@ -13389,7 +13549,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="28" customFormat="1" ht="38.4" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="25" spans="1:12" s="28" customFormat="1" ht="38.4" customHeight="1" outlineLevel="1">
       <c r="A25" s="50"/>
       <c r="B25" s="53"/>
       <c r="C25" s="27" t="s">
@@ -13405,7 +13565,7 @@
       <c r="K25" s="43"/>
       <c r="L25" s="43"/>
     </row>
-    <row r="26" spans="1:12" s="28" customFormat="1" ht="38.4" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="26" spans="1:12" s="28" customFormat="1" ht="38.4" customHeight="1" outlineLevel="1">
       <c r="A26" s="50"/>
       <c r="B26" s="53"/>
       <c r="C26" s="27" t="s">
@@ -13421,7 +13581,7 @@
       <c r="K26" s="43"/>
       <c r="L26" s="43"/>
     </row>
-    <row r="27" spans="1:12" s="28" customFormat="1" ht="38.4" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="27" spans="1:12" s="28" customFormat="1" ht="38.4" customHeight="1" outlineLevel="1">
       <c r="A27" s="50"/>
       <c r="B27" s="53"/>
       <c r="C27" s="27" t="s">
@@ -13437,7 +13597,7 @@
       <c r="K27" s="43"/>
       <c r="L27" s="43"/>
     </row>
-    <row r="28" spans="1:12" s="28" customFormat="1" ht="38.4" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="28" spans="1:12" s="28" customFormat="1" ht="38.4" customHeight="1" outlineLevel="1">
       <c r="A28" s="50"/>
       <c r="B28" s="53"/>
       <c r="C28" s="27" t="s">
@@ -13453,7 +13613,7 @@
       <c r="K28" s="43"/>
       <c r="L28" s="43"/>
     </row>
-    <row r="29" spans="1:12" s="28" customFormat="1" ht="38.4" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="29" spans="1:12" s="28" customFormat="1" ht="38.4" customHeight="1" outlineLevel="1">
       <c r="A29" s="51"/>
       <c r="B29" s="54"/>
       <c r="C29" s="27" t="s">
@@ -13469,7 +13629,7 @@
       <c r="K29" s="44"/>
       <c r="L29" s="44"/>
     </row>
-    <row r="30" spans="1:12" s="12" customFormat="1" ht="13.2" collapsed="1">
+    <row r="30" spans="1:12" s="12" customFormat="1" ht="13.2">
       <c r="A30" s="35" t="s">
         <v>85</v>
       </c>
@@ -13489,7 +13649,7 @@
       <c r="K30" s="33"/>
       <c r="L30" s="33"/>
     </row>
-    <row r="31" spans="1:12" s="28" customFormat="1" ht="42" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="31" spans="1:12" s="28" customFormat="1" ht="42" customHeight="1" outlineLevel="1">
       <c r="A31" s="88"/>
       <c r="B31" s="52" t="s">
         <v>98</v>
@@ -13523,7 +13683,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="28" customFormat="1" ht="42" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="32" spans="1:12" s="28" customFormat="1" ht="42" customHeight="1" outlineLevel="1">
       <c r="A32" s="89"/>
       <c r="B32" s="53"/>
       <c r="C32" s="27" t="s">
@@ -13539,7 +13699,7 @@
       <c r="K32" s="43"/>
       <c r="L32" s="43"/>
     </row>
-    <row r="33" spans="1:47" s="28" customFormat="1" ht="42" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="33" spans="1:47" s="28" customFormat="1" ht="42" customHeight="1" outlineLevel="1">
       <c r="A33" s="89"/>
       <c r="B33" s="53"/>
       <c r="C33" s="27" t="s">
@@ -13555,7 +13715,7 @@
       <c r="K33" s="43"/>
       <c r="L33" s="43"/>
     </row>
-    <row r="34" spans="1:47" s="28" customFormat="1" ht="42" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="34" spans="1:47" s="28" customFormat="1" ht="42" customHeight="1" outlineLevel="1">
       <c r="A34" s="89"/>
       <c r="B34" s="53"/>
       <c r="C34" s="27" t="s">
@@ -13571,7 +13731,7 @@
       <c r="K34" s="43"/>
       <c r="L34" s="43"/>
     </row>
-    <row r="35" spans="1:47" s="28" customFormat="1" ht="42" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="35" spans="1:47" s="28" customFormat="1" ht="42" customHeight="1" outlineLevel="1">
       <c r="A35" s="89"/>
       <c r="B35" s="53"/>
       <c r="C35" s="27" t="s">
@@ -13587,7 +13747,7 @@
       <c r="K35" s="43"/>
       <c r="L35" s="43"/>
     </row>
-    <row r="36" spans="1:47" s="28" customFormat="1" ht="42" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="36" spans="1:47" s="28" customFormat="1" ht="42" customHeight="1" outlineLevel="1">
       <c r="A36" s="90"/>
       <c r="B36" s="54"/>
       <c r="C36" s="27" t="s">
@@ -13603,7 +13763,7 @@
       <c r="K36" s="44"/>
       <c r="L36" s="44"/>
     </row>
-    <row r="37" spans="1:47" collapsed="1">
+    <row r="37" spans="1:47">
       <c r="A37" s="29"/>
       <c r="B37" s="29"/>
       <c r="C37" s="29"/>
@@ -32182,7 +32342,7 @@
   <dimension ref="A1:AU139"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" outlineLevelRow="1"/>
@@ -38341,8 +38501,8 @@
   </sheetPr>
   <dimension ref="A1:AU143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" outlineLevelRow="1"/>
@@ -44503,10 +44663,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:AU135"/>
+  <dimension ref="A1:AU141"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24:D26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" outlineLevelRow="1"/>
@@ -44514,7 +44674,7 @@
     <col min="1" max="1" width="16.88671875" style="30" customWidth="1"/>
     <col min="2" max="2" width="25.88671875" style="30" customWidth="1"/>
     <col min="3" max="3" width="34" style="30" customWidth="1"/>
-    <col min="4" max="4" width="59.33203125" style="30" customWidth="1"/>
+    <col min="4" max="4" width="65.5546875" style="30" customWidth="1"/>
     <col min="5" max="5" width="31.6640625" style="30" customWidth="1"/>
     <col min="6" max="6" width="13.109375" style="30" customWidth="1"/>
     <col min="7" max="7" width="16" style="30" customWidth="1"/>
@@ -44718,7 +44878,7 @@
         <v>Build1</v>
       </c>
       <c r="B14" s="19">
-        <f t="shared" ref="B14:G14" si="0">COUNTIF($L$23:$L$48462,B13)</f>
+        <f t="shared" ref="B14:G14" si="0">COUNTIF($L$23:$L$48468,B13)</f>
         <v>0</v>
       </c>
       <c r="C14" s="19">
@@ -44753,7 +44913,7 @@
         <v>Build2</v>
       </c>
       <c r="B15" s="19">
-        <f t="shared" ref="B15:G15" si="1">COUNTIF($K$23:$K$48462,B13)</f>
+        <f t="shared" ref="B15:G15" si="1">COUNTIF($K$23:$K$48468,B13)</f>
         <v>0</v>
       </c>
       <c r="C15" s="19">
@@ -44788,7 +44948,7 @@
         <v>Build3</v>
       </c>
       <c r="B16" s="19">
-        <f t="shared" ref="B16:G16" si="2">COUNTIF($J$23:$J$48462,B13)</f>
+        <f t="shared" ref="B16:G16" si="2">COUNTIF($J$23:$J$48468,B13)</f>
         <v>0</v>
       </c>
       <c r="C16" s="19">
@@ -44817,33 +44977,33 @@
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
     </row>
-    <row r="17" spans="1:47" s="13" customFormat="1" ht="20.25" customHeight="1">
+    <row r="17" spans="1:12" s="13" customFormat="1" ht="20.25" customHeight="1">
       <c r="A17" s="18" t="str">
         <f>I22</f>
         <v>Build4</v>
       </c>
       <c r="B17" s="19">
-        <f>COUNTIF($I$23:$I$48462,B13)</f>
+        <f>COUNTIF($I$23:$I$48468,B13)</f>
         <v>0</v>
       </c>
       <c r="C17" s="19">
-        <f>COUNTIF($I$23:$I$48462,C16)</f>
+        <f>COUNTIF($I$23:$I$48468,C16)</f>
         <v>0</v>
       </c>
       <c r="D17" s="19">
-        <f>COUNTIF($I$23:$I$48462,D13)</f>
+        <f>COUNTIF($I$23:$I$48468,D13)</f>
         <v>0</v>
       </c>
       <c r="E17" s="19">
-        <f>COUNTIF($I$23:$I$48462,E13)</f>
+        <f>COUNTIF($I$23:$I$48468,E13)</f>
         <v>0</v>
       </c>
       <c r="F17" s="19">
-        <f>COUNTIF($I$23:$I$48462,F13)</f>
+        <f>COUNTIF($I$23:$I$48468,F13)</f>
         <v>0</v>
       </c>
       <c r="G17" s="19">
-        <f>COUNTIF($I$23:$I$48462,G13)</f>
+        <f>COUNTIF($I$23:$I$48468,G13)</f>
         <v>0</v>
       </c>
       <c r="H17" s="20"/>
@@ -44852,13 +45012,13 @@
       <c r="K17" s="20"/>
       <c r="L17" s="20"/>
     </row>
-    <row r="18" spans="1:47" s="13" customFormat="1" ht="22.5" customHeight="1">
+    <row r="18" spans="1:12" s="13" customFormat="1" ht="22.5" customHeight="1">
       <c r="A18" s="18" t="str">
         <f>H22</f>
         <v>Build5</v>
       </c>
       <c r="B18" s="19">
-        <f t="shared" ref="B18:G18" si="3">COUNTIF($H$23:$H$48462,B13)</f>
+        <f t="shared" ref="B18:G18" si="3">COUNTIF($H$23:$H$48468,B13)</f>
         <v>0</v>
       </c>
       <c r="C18" s="19">
@@ -44871,7 +45031,7 @@
       </c>
       <c r="E18" s="19">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F18" s="19">
         <f t="shared" si="3"/>
@@ -44887,7 +45047,7 @@
       <c r="K18" s="20"/>
       <c r="L18" s="20"/>
     </row>
-    <row r="19" spans="1:47" s="13" customFormat="1" ht="18.75" customHeight="1">
+    <row r="19" spans="1:12" s="13" customFormat="1" ht="18.75" customHeight="1">
       <c r="A19" s="21" t="s">
         <v>15</v>
       </c>
@@ -44905,7 +45065,7 @@
       </c>
       <c r="E19" s="22">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F19" s="22">
         <f t="shared" si="4"/>
@@ -44921,7 +45081,7 @@
       <c r="K19" s="20"/>
       <c r="L19" s="20"/>
     </row>
-    <row r="20" spans="1:47" s="13" customFormat="1" ht="11.4">
+    <row r="20" spans="1:12" s="13" customFormat="1" ht="11.4">
       <c r="A20" s="23"/>
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
@@ -44935,7 +45095,7 @@
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
     </row>
-    <row r="21" spans="1:47" s="24" customFormat="1" ht="15" customHeight="1">
+    <row r="21" spans="1:12" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="D21" s="25"/>
       <c r="E21" s="25"/>
       <c r="F21" s="25"/>
@@ -44948,7 +45108,7 @@
       <c r="K21" s="78"/>
       <c r="L21" s="78"/>
     </row>
-    <row r="22" spans="1:47" s="24" customFormat="1" ht="13.2">
+    <row r="22" spans="1:12" s="24" customFormat="1" ht="13.2">
       <c r="A22" s="26" t="s">
         <v>16</v>
       </c>
@@ -44986,11 +45146,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:47" s="12" customFormat="1" ht="13.2">
+    <row r="23" spans="1:12" s="12" customFormat="1" ht="13.2">
       <c r="A23" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="62"/>
+      <c r="B23" s="62" t="s">
+        <v>201</v>
+      </c>
       <c r="C23" s="63"/>
       <c r="D23" s="64"/>
       <c r="E23" s="31"/>
@@ -45004,1288 +45166,541 @@
       <c r="K23" s="33"/>
       <c r="L23" s="33"/>
     </row>
-    <row r="24" spans="1:47" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+    <row r="24" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
       <c r="A24" s="72"/>
       <c r="B24" s="68" t="s">
         <v>164</v>
       </c>
-      <c r="C24" s="39"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="93"/>
+      <c r="C24" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="D24" s="73" t="s">
+        <v>217</v>
+      </c>
+      <c r="E24" s="94"/>
       <c r="F24" s="80" t="s">
         <v>28</v>
       </c>
       <c r="G24" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="H24" s="80" t="s">
+      <c r="H24" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="I24" s="80" t="s">
+      <c r="I24" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="J24" s="80" t="s">
+      <c r="J24" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="K24" s="80" t="s">
+      <c r="K24" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="L24" s="80" t="s">
+      <c r="L24" s="65" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:47" s="28" customFormat="1" ht="36" customHeight="1" outlineLevel="1">
+    <row r="25" spans="1:12" s="28" customFormat="1" ht="36" customHeight="1" outlineLevel="1">
       <c r="A25" s="72"/>
       <c r="B25" s="68"/>
-      <c r="C25" s="27"/>
+      <c r="C25" s="27" t="s">
+        <v>198</v>
+      </c>
       <c r="D25" s="73"/>
-      <c r="E25" s="93"/>
+      <c r="E25" s="94"/>
       <c r="F25" s="80"/>
       <c r="G25" s="80"/>
-      <c r="H25" s="80"/>
-      <c r="I25" s="80"/>
-      <c r="J25" s="80"/>
-      <c r="K25" s="80"/>
-      <c r="L25" s="80"/>
-    </row>
-    <row r="26" spans="1:47" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="H25" s="66"/>
+      <c r="I25" s="66"/>
+      <c r="J25" s="66"/>
+      <c r="K25" s="66"/>
+      <c r="L25" s="66"/>
+    </row>
+    <row r="26" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
       <c r="A26" s="72"/>
       <c r="B26" s="68"/>
-      <c r="C26" s="27"/>
+      <c r="C26" s="27" t="s">
+        <v>199</v>
+      </c>
       <c r="D26" s="73"/>
-      <c r="E26" s="93"/>
+      <c r="E26" s="94"/>
       <c r="F26" s="80"/>
       <c r="G26" s="80"/>
-      <c r="H26" s="80"/>
-      <c r="I26" s="80"/>
-      <c r="J26" s="80"/>
-      <c r="K26" s="80"/>
-      <c r="L26" s="80"/>
-    </row>
-    <row r="27" spans="1:47">
-      <c r="A27" s="29"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="29"/>
-      <c r="O27" s="29"/>
-      <c r="P27" s="29"/>
-      <c r="Q27" s="29"/>
-      <c r="R27" s="29"/>
-      <c r="S27" s="29"/>
-      <c r="T27" s="29"/>
-      <c r="U27" s="29"/>
-      <c r="V27" s="29"/>
-      <c r="W27" s="29"/>
-      <c r="X27" s="29"/>
-      <c r="Y27" s="29"/>
-      <c r="Z27" s="29"/>
-      <c r="AA27" s="29"/>
-      <c r="AB27" s="29"/>
-      <c r="AC27" s="29"/>
-      <c r="AD27" s="29"/>
-      <c r="AE27" s="29"/>
-      <c r="AF27" s="29"/>
-      <c r="AG27" s="29"/>
-      <c r="AH27" s="29"/>
-      <c r="AI27" s="29"/>
-      <c r="AJ27" s="29"/>
-      <c r="AK27" s="29"/>
-      <c r="AL27" s="29"/>
-      <c r="AM27" s="29"/>
-      <c r="AN27" s="29"/>
-      <c r="AO27" s="29"/>
-      <c r="AP27" s="29"/>
-      <c r="AQ27" s="29"/>
-      <c r="AR27" s="29"/>
-      <c r="AS27" s="29"/>
-      <c r="AT27" s="29"/>
-      <c r="AU27" s="29"/>
-    </row>
-    <row r="28" spans="1:47">
-      <c r="A28" s="29"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
-      <c r="O28" s="29"/>
-      <c r="P28" s="29"/>
-      <c r="Q28" s="29"/>
-      <c r="R28" s="29"/>
-      <c r="S28" s="29"/>
-      <c r="T28" s="29"/>
-      <c r="U28" s="29"/>
-      <c r="V28" s="29"/>
-      <c r="W28" s="29"/>
-      <c r="X28" s="29"/>
-      <c r="Y28" s="29"/>
-      <c r="Z28" s="29"/>
-      <c r="AA28" s="29"/>
-      <c r="AB28" s="29"/>
-      <c r="AC28" s="29"/>
-      <c r="AD28" s="29"/>
-      <c r="AE28" s="29"/>
-      <c r="AF28" s="29"/>
-      <c r="AG28" s="29"/>
-      <c r="AH28" s="29"/>
-      <c r="AI28" s="29"/>
-      <c r="AJ28" s="29"/>
-      <c r="AK28" s="29"/>
-      <c r="AL28" s="29"/>
-      <c r="AM28" s="29"/>
-      <c r="AN28" s="29"/>
-      <c r="AO28" s="29"/>
-      <c r="AP28" s="29"/>
-      <c r="AQ28" s="29"/>
-      <c r="AR28" s="29"/>
-      <c r="AS28" s="29"/>
-      <c r="AT28" s="29"/>
-      <c r="AU28" s="29"/>
-    </row>
-    <row r="29" spans="1:47">
-      <c r="A29" s="29"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="29"/>
-      <c r="N29" s="29"/>
-      <c r="O29" s="29"/>
-      <c r="P29" s="29"/>
-      <c r="Q29" s="29"/>
-      <c r="R29" s="29"/>
-      <c r="S29" s="29"/>
-      <c r="T29" s="29"/>
-      <c r="U29" s="29"/>
-      <c r="V29" s="29"/>
-      <c r="W29" s="29"/>
-      <c r="X29" s="29"/>
-      <c r="Y29" s="29"/>
-      <c r="Z29" s="29"/>
-      <c r="AA29" s="29"/>
-      <c r="AB29" s="29"/>
-      <c r="AC29" s="29"/>
-      <c r="AD29" s="29"/>
-      <c r="AE29" s="29"/>
-      <c r="AF29" s="29"/>
-      <c r="AG29" s="29"/>
-      <c r="AH29" s="29"/>
-      <c r="AI29" s="29"/>
-      <c r="AJ29" s="29"/>
-      <c r="AK29" s="29"/>
-      <c r="AL29" s="29"/>
-      <c r="AM29" s="29"/>
-      <c r="AN29" s="29"/>
-      <c r="AO29" s="29"/>
-      <c r="AP29" s="29"/>
-      <c r="AQ29" s="29"/>
-      <c r="AR29" s="29"/>
-      <c r="AS29" s="29"/>
-      <c r="AT29" s="29"/>
-      <c r="AU29" s="29"/>
-    </row>
-    <row r="30" spans="1:47">
-      <c r="A30" s="29"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="29"/>
-      <c r="O30" s="29"/>
-      <c r="P30" s="29"/>
-      <c r="Q30" s="29"/>
-      <c r="R30" s="29"/>
-      <c r="S30" s="29"/>
-      <c r="T30" s="29"/>
-      <c r="U30" s="29"/>
-      <c r="V30" s="29"/>
-      <c r="W30" s="29"/>
-      <c r="X30" s="29"/>
-      <c r="Y30" s="29"/>
-      <c r="Z30" s="29"/>
-      <c r="AA30" s="29"/>
-      <c r="AB30" s="29"/>
-      <c r="AC30" s="29"/>
-      <c r="AD30" s="29"/>
-      <c r="AE30" s="29"/>
-      <c r="AF30" s="29"/>
-      <c r="AG30" s="29"/>
-      <c r="AH30" s="29"/>
-      <c r="AI30" s="29"/>
-      <c r="AJ30" s="29"/>
-      <c r="AK30" s="29"/>
-      <c r="AL30" s="29"/>
-      <c r="AM30" s="29"/>
-      <c r="AN30" s="29"/>
-      <c r="AO30" s="29"/>
-      <c r="AP30" s="29"/>
-      <c r="AQ30" s="29"/>
-      <c r="AR30" s="29"/>
-      <c r="AS30" s="29"/>
-      <c r="AT30" s="29"/>
-      <c r="AU30" s="29"/>
-    </row>
-    <row r="31" spans="1:47">
-      <c r="A31" s="29"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="29"/>
-      <c r="O31" s="29"/>
-      <c r="P31" s="29"/>
-      <c r="Q31" s="29"/>
-      <c r="R31" s="29"/>
-      <c r="S31" s="29"/>
-      <c r="T31" s="29"/>
-      <c r="U31" s="29"/>
-      <c r="V31" s="29"/>
-      <c r="W31" s="29"/>
-      <c r="X31" s="29"/>
-      <c r="Y31" s="29"/>
-      <c r="Z31" s="29"/>
-      <c r="AA31" s="29"/>
-      <c r="AB31" s="29"/>
-      <c r="AC31" s="29"/>
-      <c r="AD31" s="29"/>
-      <c r="AE31" s="29"/>
-      <c r="AF31" s="29"/>
-      <c r="AG31" s="29"/>
-      <c r="AH31" s="29"/>
-      <c r="AI31" s="29"/>
-      <c r="AJ31" s="29"/>
-      <c r="AK31" s="29"/>
-      <c r="AL31" s="29"/>
-      <c r="AM31" s="29"/>
-      <c r="AN31" s="29"/>
-      <c r="AO31" s="29"/>
-      <c r="AP31" s="29"/>
-      <c r="AQ31" s="29"/>
-      <c r="AR31" s="29"/>
-      <c r="AS31" s="29"/>
-      <c r="AT31" s="29"/>
-      <c r="AU31" s="29"/>
-    </row>
-    <row r="32" spans="1:47">
-      <c r="A32" s="29"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
-      <c r="O32" s="29"/>
-      <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
-      <c r="R32" s="29"/>
-      <c r="S32" s="29"/>
-      <c r="T32" s="29"/>
-      <c r="U32" s="29"/>
-      <c r="V32" s="29"/>
-      <c r="W32" s="29"/>
-      <c r="X32" s="29"/>
-      <c r="Y32" s="29"/>
-      <c r="Z32" s="29"/>
-      <c r="AA32" s="29"/>
-      <c r="AB32" s="29"/>
-      <c r="AC32" s="29"/>
-      <c r="AD32" s="29"/>
-      <c r="AE32" s="29"/>
-      <c r="AF32" s="29"/>
-      <c r="AG32" s="29"/>
-      <c r="AH32" s="29"/>
-      <c r="AI32" s="29"/>
-      <c r="AJ32" s="29"/>
-      <c r="AK32" s="29"/>
-      <c r="AL32" s="29"/>
-      <c r="AM32" s="29"/>
-      <c r="AN32" s="29"/>
-      <c r="AO32" s="29"/>
-      <c r="AP32" s="29"/>
-      <c r="AQ32" s="29"/>
-      <c r="AR32" s="29"/>
-      <c r="AS32" s="29"/>
-      <c r="AT32" s="29"/>
-      <c r="AU32" s="29"/>
-    </row>
-    <row r="33" spans="1:47">
-      <c r="A33" s="29"/>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="29"/>
-      <c r="N33" s="29"/>
-      <c r="O33" s="29"/>
-      <c r="P33" s="29"/>
-      <c r="Q33" s="29"/>
-      <c r="R33" s="29"/>
-      <c r="S33" s="29"/>
-      <c r="T33" s="29"/>
-      <c r="U33" s="29"/>
-      <c r="V33" s="29"/>
-      <c r="W33" s="29"/>
-      <c r="X33" s="29"/>
-      <c r="Y33" s="29"/>
-      <c r="Z33" s="29"/>
-      <c r="AA33" s="29"/>
-      <c r="AB33" s="29"/>
-      <c r="AC33" s="29"/>
-      <c r="AD33" s="29"/>
-      <c r="AE33" s="29"/>
-      <c r="AF33" s="29"/>
-      <c r="AG33" s="29"/>
-      <c r="AH33" s="29"/>
-      <c r="AI33" s="29"/>
-      <c r="AJ33" s="29"/>
-      <c r="AK33" s="29"/>
-      <c r="AL33" s="29"/>
-      <c r="AM33" s="29"/>
-      <c r="AN33" s="29"/>
-      <c r="AO33" s="29"/>
-      <c r="AP33" s="29"/>
-      <c r="AQ33" s="29"/>
-      <c r="AR33" s="29"/>
-      <c r="AS33" s="29"/>
-      <c r="AT33" s="29"/>
-      <c r="AU33" s="29"/>
-    </row>
-    <row r="34" spans="1:47">
-      <c r="A34" s="29"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="29"/>
-      <c r="J34" s="29"/>
-      <c r="K34" s="29"/>
-      <c r="L34" s="29"/>
-      <c r="M34" s="29"/>
-      <c r="N34" s="29"/>
-      <c r="O34" s="29"/>
-      <c r="P34" s="29"/>
-      <c r="Q34" s="29"/>
-      <c r="R34" s="29"/>
-      <c r="S34" s="29"/>
-      <c r="T34" s="29"/>
-      <c r="U34" s="29"/>
-      <c r="V34" s="29"/>
-      <c r="W34" s="29"/>
-      <c r="X34" s="29"/>
-      <c r="Y34" s="29"/>
-      <c r="Z34" s="29"/>
-      <c r="AA34" s="29"/>
-      <c r="AB34" s="29"/>
-      <c r="AC34" s="29"/>
-      <c r="AD34" s="29"/>
-      <c r="AE34" s="29"/>
-      <c r="AF34" s="29"/>
-      <c r="AG34" s="29"/>
-      <c r="AH34" s="29"/>
-      <c r="AI34" s="29"/>
-      <c r="AJ34" s="29"/>
-      <c r="AK34" s="29"/>
-      <c r="AL34" s="29"/>
-      <c r="AM34" s="29"/>
-      <c r="AN34" s="29"/>
-      <c r="AO34" s="29"/>
-      <c r="AP34" s="29"/>
-      <c r="AQ34" s="29"/>
-      <c r="AR34" s="29"/>
-      <c r="AS34" s="29"/>
-      <c r="AT34" s="29"/>
-      <c r="AU34" s="29"/>
-    </row>
-    <row r="35" spans="1:47">
-      <c r="A35" s="29"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="29"/>
-      <c r="J35" s="29"/>
-      <c r="K35" s="29"/>
-      <c r="L35" s="29"/>
-      <c r="M35" s="29"/>
-      <c r="N35" s="29"/>
-      <c r="O35" s="29"/>
-      <c r="P35" s="29"/>
-      <c r="Q35" s="29"/>
-      <c r="R35" s="29"/>
-      <c r="S35" s="29"/>
-      <c r="T35" s="29"/>
-      <c r="U35" s="29"/>
-      <c r="V35" s="29"/>
-      <c r="W35" s="29"/>
-      <c r="X35" s="29"/>
-      <c r="Y35" s="29"/>
-      <c r="Z35" s="29"/>
-      <c r="AA35" s="29"/>
-      <c r="AB35" s="29"/>
-      <c r="AC35" s="29"/>
-      <c r="AD35" s="29"/>
-      <c r="AE35" s="29"/>
-      <c r="AF35" s="29"/>
-      <c r="AG35" s="29"/>
-      <c r="AH35" s="29"/>
-      <c r="AI35" s="29"/>
-      <c r="AJ35" s="29"/>
-      <c r="AK35" s="29"/>
-      <c r="AL35" s="29"/>
-      <c r="AM35" s="29"/>
-      <c r="AN35" s="29"/>
-      <c r="AO35" s="29"/>
-      <c r="AP35" s="29"/>
-      <c r="AQ35" s="29"/>
-      <c r="AR35" s="29"/>
-      <c r="AS35" s="29"/>
-      <c r="AT35" s="29"/>
-      <c r="AU35" s="29"/>
-    </row>
-    <row r="36" spans="1:47">
-      <c r="A36" s="29"/>
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="29"/>
-      <c r="J36" s="29"/>
-      <c r="K36" s="29"/>
-      <c r="L36" s="29"/>
-      <c r="M36" s="29"/>
-      <c r="N36" s="29"/>
-      <c r="O36" s="29"/>
-      <c r="P36" s="29"/>
-      <c r="Q36" s="29"/>
-      <c r="R36" s="29"/>
-      <c r="S36" s="29"/>
-      <c r="T36" s="29"/>
-      <c r="U36" s="29"/>
-      <c r="V36" s="29"/>
-      <c r="W36" s="29"/>
-      <c r="X36" s="29"/>
-      <c r="Y36" s="29"/>
-      <c r="Z36" s="29"/>
-      <c r="AA36" s="29"/>
-      <c r="AB36" s="29"/>
-      <c r="AC36" s="29"/>
-      <c r="AD36" s="29"/>
-      <c r="AE36" s="29"/>
-      <c r="AF36" s="29"/>
-      <c r="AG36" s="29"/>
-      <c r="AH36" s="29"/>
-      <c r="AI36" s="29"/>
-      <c r="AJ36" s="29"/>
-      <c r="AK36" s="29"/>
-      <c r="AL36" s="29"/>
-      <c r="AM36" s="29"/>
-      <c r="AN36" s="29"/>
-      <c r="AO36" s="29"/>
-      <c r="AP36" s="29"/>
-      <c r="AQ36" s="29"/>
-      <c r="AR36" s="29"/>
-      <c r="AS36" s="29"/>
-      <c r="AT36" s="29"/>
-      <c r="AU36" s="29"/>
-    </row>
-    <row r="37" spans="1:47">
-      <c r="A37" s="29"/>
-      <c r="B37" s="29"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="29"/>
-      <c r="N37" s="29"/>
-      <c r="O37" s="29"/>
-      <c r="P37" s="29"/>
-      <c r="Q37" s="29"/>
-      <c r="R37" s="29"/>
-      <c r="S37" s="29"/>
-      <c r="T37" s="29"/>
-      <c r="U37" s="29"/>
-      <c r="V37" s="29"/>
-      <c r="W37" s="29"/>
-      <c r="X37" s="29"/>
-      <c r="Y37" s="29"/>
-      <c r="Z37" s="29"/>
-      <c r="AA37" s="29"/>
-      <c r="AB37" s="29"/>
-      <c r="AC37" s="29"/>
-      <c r="AD37" s="29"/>
-      <c r="AE37" s="29"/>
-      <c r="AF37" s="29"/>
-      <c r="AG37" s="29"/>
-      <c r="AH37" s="29"/>
-      <c r="AI37" s="29"/>
-      <c r="AJ37" s="29"/>
-      <c r="AK37" s="29"/>
-      <c r="AL37" s="29"/>
-      <c r="AM37" s="29"/>
-      <c r="AN37" s="29"/>
-      <c r="AO37" s="29"/>
-      <c r="AP37" s="29"/>
-      <c r="AQ37" s="29"/>
-      <c r="AR37" s="29"/>
-      <c r="AS37" s="29"/>
-      <c r="AT37" s="29"/>
-      <c r="AU37" s="29"/>
-    </row>
-    <row r="38" spans="1:47">
-      <c r="A38" s="29"/>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
-      <c r="N38" s="29"/>
-      <c r="O38" s="29"/>
-      <c r="P38" s="29"/>
-      <c r="Q38" s="29"/>
-      <c r="R38" s="29"/>
-      <c r="S38" s="29"/>
-      <c r="T38" s="29"/>
-      <c r="U38" s="29"/>
-      <c r="V38" s="29"/>
-      <c r="W38" s="29"/>
-      <c r="X38" s="29"/>
-      <c r="Y38" s="29"/>
-      <c r="Z38" s="29"/>
-      <c r="AA38" s="29"/>
-      <c r="AB38" s="29"/>
-      <c r="AC38" s="29"/>
-      <c r="AD38" s="29"/>
-      <c r="AE38" s="29"/>
-      <c r="AF38" s="29"/>
-      <c r="AG38" s="29"/>
-      <c r="AH38" s="29"/>
-      <c r="AI38" s="29"/>
-      <c r="AJ38" s="29"/>
-      <c r="AK38" s="29"/>
-      <c r="AL38" s="29"/>
-      <c r="AM38" s="29"/>
-      <c r="AN38" s="29"/>
-      <c r="AO38" s="29"/>
-      <c r="AP38" s="29"/>
-      <c r="AQ38" s="29"/>
-      <c r="AR38" s="29"/>
-      <c r="AS38" s="29"/>
-      <c r="AT38" s="29"/>
-      <c r="AU38" s="29"/>
-    </row>
-    <row r="39" spans="1:47">
-      <c r="A39" s="29"/>
-      <c r="B39" s="29"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="29"/>
-      <c r="J39" s="29"/>
-      <c r="K39" s="29"/>
-      <c r="L39" s="29"/>
-      <c r="M39" s="29"/>
-      <c r="N39" s="29"/>
-      <c r="O39" s="29"/>
-      <c r="P39" s="29"/>
-      <c r="Q39" s="29"/>
-      <c r="R39" s="29"/>
-      <c r="S39" s="29"/>
-      <c r="T39" s="29"/>
-      <c r="U39" s="29"/>
-      <c r="V39" s="29"/>
-      <c r="W39" s="29"/>
-      <c r="X39" s="29"/>
-      <c r="Y39" s="29"/>
-      <c r="Z39" s="29"/>
-      <c r="AA39" s="29"/>
-      <c r="AB39" s="29"/>
-      <c r="AC39" s="29"/>
-      <c r="AD39" s="29"/>
-      <c r="AE39" s="29"/>
-      <c r="AF39" s="29"/>
-      <c r="AG39" s="29"/>
-      <c r="AH39" s="29"/>
-      <c r="AI39" s="29"/>
-      <c r="AJ39" s="29"/>
-      <c r="AK39" s="29"/>
-      <c r="AL39" s="29"/>
-      <c r="AM39" s="29"/>
-      <c r="AN39" s="29"/>
-      <c r="AO39" s="29"/>
-      <c r="AP39" s="29"/>
-      <c r="AQ39" s="29"/>
-      <c r="AR39" s="29"/>
-      <c r="AS39" s="29"/>
-      <c r="AT39" s="29"/>
-      <c r="AU39" s="29"/>
-    </row>
-    <row r="40" spans="1:47">
-      <c r="A40" s="29"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
-      <c r="N40" s="29"/>
-      <c r="O40" s="29"/>
-      <c r="P40" s="29"/>
-      <c r="Q40" s="29"/>
-      <c r="R40" s="29"/>
-      <c r="S40" s="29"/>
-      <c r="T40" s="29"/>
-      <c r="U40" s="29"/>
-      <c r="V40" s="29"/>
-      <c r="W40" s="29"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="29"/>
-      <c r="AA40" s="29"/>
-      <c r="AB40" s="29"/>
-      <c r="AC40" s="29"/>
-      <c r="AD40" s="29"/>
-      <c r="AE40" s="29"/>
-      <c r="AF40" s="29"/>
-      <c r="AG40" s="29"/>
-      <c r="AH40" s="29"/>
-      <c r="AI40" s="29"/>
-      <c r="AJ40" s="29"/>
-      <c r="AK40" s="29"/>
-      <c r="AL40" s="29"/>
-      <c r="AM40" s="29"/>
-      <c r="AN40" s="29"/>
-      <c r="AO40" s="29"/>
-      <c r="AP40" s="29"/>
-      <c r="AQ40" s="29"/>
-      <c r="AR40" s="29"/>
-      <c r="AS40" s="29"/>
-      <c r="AT40" s="29"/>
-      <c r="AU40" s="29"/>
-    </row>
-    <row r="41" spans="1:47">
-      <c r="A41" s="29"/>
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="29"/>
-      <c r="J41" s="29"/>
-      <c r="K41" s="29"/>
-      <c r="L41" s="29"/>
-      <c r="M41" s="29"/>
-      <c r="N41" s="29"/>
-      <c r="O41" s="29"/>
-      <c r="P41" s="29"/>
-      <c r="Q41" s="29"/>
-      <c r="R41" s="29"/>
-      <c r="S41" s="29"/>
-      <c r="T41" s="29"/>
-      <c r="U41" s="29"/>
-      <c r="V41" s="29"/>
-      <c r="W41" s="29"/>
-      <c r="X41" s="29"/>
-      <c r="Y41" s="29"/>
-      <c r="Z41" s="29"/>
-      <c r="AA41" s="29"/>
-      <c r="AB41" s="29"/>
-      <c r="AC41" s="29"/>
-      <c r="AD41" s="29"/>
-      <c r="AE41" s="29"/>
-      <c r="AF41" s="29"/>
-      <c r="AG41" s="29"/>
-      <c r="AH41" s="29"/>
-      <c r="AI41" s="29"/>
-      <c r="AJ41" s="29"/>
-      <c r="AK41" s="29"/>
-      <c r="AL41" s="29"/>
-      <c r="AM41" s="29"/>
-      <c r="AN41" s="29"/>
-      <c r="AO41" s="29"/>
-      <c r="AP41" s="29"/>
-      <c r="AQ41" s="29"/>
-      <c r="AR41" s="29"/>
-      <c r="AS41" s="29"/>
-      <c r="AT41" s="29"/>
-      <c r="AU41" s="29"/>
-    </row>
-    <row r="42" spans="1:47">
-      <c r="A42" s="29"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
-      <c r="O42" s="29"/>
-      <c r="P42" s="29"/>
-      <c r="Q42" s="29"/>
-      <c r="R42" s="29"/>
-      <c r="S42" s="29"/>
-      <c r="T42" s="29"/>
-      <c r="U42" s="29"/>
-      <c r="V42" s="29"/>
-      <c r="W42" s="29"/>
-      <c r="X42" s="29"/>
-      <c r="Y42" s="29"/>
-      <c r="Z42" s="29"/>
-      <c r="AA42" s="29"/>
-      <c r="AB42" s="29"/>
-      <c r="AC42" s="29"/>
-      <c r="AD42" s="29"/>
-      <c r="AE42" s="29"/>
-      <c r="AF42" s="29"/>
-      <c r="AG42" s="29"/>
-      <c r="AH42" s="29"/>
-      <c r="AI42" s="29"/>
-      <c r="AJ42" s="29"/>
-      <c r="AK42" s="29"/>
-      <c r="AL42" s="29"/>
-      <c r="AM42" s="29"/>
-      <c r="AN42" s="29"/>
-      <c r="AO42" s="29"/>
-      <c r="AP42" s="29"/>
-      <c r="AQ42" s="29"/>
-      <c r="AR42" s="29"/>
-      <c r="AS42" s="29"/>
-      <c r="AT42" s="29"/>
-      <c r="AU42" s="29"/>
-    </row>
-    <row r="43" spans="1:47">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
-      <c r="K43" s="29"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="29"/>
-      <c r="N43" s="29"/>
-      <c r="O43" s="29"/>
-      <c r="P43" s="29"/>
-      <c r="Q43" s="29"/>
-      <c r="R43" s="29"/>
-      <c r="S43" s="29"/>
-      <c r="T43" s="29"/>
-      <c r="U43" s="29"/>
-      <c r="V43" s="29"/>
-      <c r="W43" s="29"/>
-      <c r="X43" s="29"/>
-      <c r="Y43" s="29"/>
-      <c r="Z43" s="29"/>
-      <c r="AA43" s="29"/>
-      <c r="AB43" s="29"/>
-      <c r="AC43" s="29"/>
-      <c r="AD43" s="29"/>
-      <c r="AE43" s="29"/>
-      <c r="AF43" s="29"/>
-      <c r="AG43" s="29"/>
-      <c r="AH43" s="29"/>
-      <c r="AI43" s="29"/>
-      <c r="AJ43" s="29"/>
-      <c r="AK43" s="29"/>
-      <c r="AL43" s="29"/>
-      <c r="AM43" s="29"/>
-      <c r="AN43" s="29"/>
-      <c r="AO43" s="29"/>
-      <c r="AP43" s="29"/>
-      <c r="AQ43" s="29"/>
-      <c r="AR43" s="29"/>
-      <c r="AS43" s="29"/>
-      <c r="AT43" s="29"/>
-      <c r="AU43" s="29"/>
-    </row>
-    <row r="44" spans="1:47">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="29"/>
-      <c r="N44" s="29"/>
-      <c r="O44" s="29"/>
-      <c r="P44" s="29"/>
-      <c r="Q44" s="29"/>
-      <c r="R44" s="29"/>
-      <c r="S44" s="29"/>
-      <c r="T44" s="29"/>
-      <c r="U44" s="29"/>
-      <c r="V44" s="29"/>
-      <c r="W44" s="29"/>
-      <c r="X44" s="29"/>
-      <c r="Y44" s="29"/>
-      <c r="Z44" s="29"/>
-      <c r="AA44" s="29"/>
-      <c r="AB44" s="29"/>
-      <c r="AC44" s="29"/>
-      <c r="AD44" s="29"/>
-      <c r="AE44" s="29"/>
-      <c r="AF44" s="29"/>
-      <c r="AG44" s="29"/>
-      <c r="AH44" s="29"/>
-      <c r="AI44" s="29"/>
-      <c r="AJ44" s="29"/>
-      <c r="AK44" s="29"/>
-      <c r="AL44" s="29"/>
-      <c r="AM44" s="29"/>
-      <c r="AN44" s="29"/>
-      <c r="AO44" s="29"/>
-      <c r="AP44" s="29"/>
-      <c r="AQ44" s="29"/>
-      <c r="AR44" s="29"/>
-      <c r="AS44" s="29"/>
-      <c r="AT44" s="29"/>
-      <c r="AU44" s="29"/>
-    </row>
-    <row r="45" spans="1:47">
-      <c r="A45" s="29"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="29"/>
-      <c r="K45" s="29"/>
-      <c r="L45" s="29"/>
-      <c r="M45" s="29"/>
-      <c r="N45" s="29"/>
-      <c r="O45" s="29"/>
-      <c r="P45" s="29"/>
-      <c r="Q45" s="29"/>
-      <c r="R45" s="29"/>
-      <c r="S45" s="29"/>
-      <c r="T45" s="29"/>
-      <c r="U45" s="29"/>
-      <c r="V45" s="29"/>
-      <c r="W45" s="29"/>
-      <c r="X45" s="29"/>
-      <c r="Y45" s="29"/>
-      <c r="Z45" s="29"/>
-      <c r="AA45" s="29"/>
-      <c r="AB45" s="29"/>
-      <c r="AC45" s="29"/>
-      <c r="AD45" s="29"/>
-      <c r="AE45" s="29"/>
-      <c r="AF45" s="29"/>
-      <c r="AG45" s="29"/>
-      <c r="AH45" s="29"/>
-      <c r="AI45" s="29"/>
-      <c r="AJ45" s="29"/>
-      <c r="AK45" s="29"/>
-      <c r="AL45" s="29"/>
-      <c r="AM45" s="29"/>
-      <c r="AN45" s="29"/>
-      <c r="AO45" s="29"/>
-      <c r="AP45" s="29"/>
-      <c r="AQ45" s="29"/>
-      <c r="AR45" s="29"/>
-      <c r="AS45" s="29"/>
-      <c r="AT45" s="29"/>
-      <c r="AU45" s="29"/>
-    </row>
-    <row r="46" spans="1:47">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="29"/>
-      <c r="H46" s="29"/>
-      <c r="I46" s="29"/>
-      <c r="J46" s="29"/>
-      <c r="K46" s="29"/>
-      <c r="L46" s="29"/>
-      <c r="M46" s="29"/>
-      <c r="N46" s="29"/>
-      <c r="O46" s="29"/>
-      <c r="P46" s="29"/>
-      <c r="Q46" s="29"/>
-      <c r="R46" s="29"/>
-      <c r="S46" s="29"/>
-      <c r="T46" s="29"/>
-      <c r="U46" s="29"/>
-      <c r="V46" s="29"/>
-      <c r="W46" s="29"/>
-      <c r="X46" s="29"/>
-      <c r="Y46" s="29"/>
-      <c r="Z46" s="29"/>
-      <c r="AA46" s="29"/>
-      <c r="AB46" s="29"/>
-      <c r="AC46" s="29"/>
-      <c r="AD46" s="29"/>
-      <c r="AE46" s="29"/>
-      <c r="AF46" s="29"/>
-      <c r="AG46" s="29"/>
-      <c r="AH46" s="29"/>
-      <c r="AI46" s="29"/>
-      <c r="AJ46" s="29"/>
-      <c r="AK46" s="29"/>
-      <c r="AL46" s="29"/>
-      <c r="AM46" s="29"/>
-      <c r="AN46" s="29"/>
-      <c r="AO46" s="29"/>
-      <c r="AP46" s="29"/>
-      <c r="AQ46" s="29"/>
-      <c r="AR46" s="29"/>
-      <c r="AS46" s="29"/>
-      <c r="AT46" s="29"/>
-      <c r="AU46" s="29"/>
-    </row>
-    <row r="47" spans="1:47">
-      <c r="A47" s="29"/>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="29"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="29"/>
-      <c r="J47" s="29"/>
-      <c r="K47" s="29"/>
-      <c r="L47" s="29"/>
-      <c r="M47" s="29"/>
-      <c r="N47" s="29"/>
-      <c r="O47" s="29"/>
-      <c r="P47" s="29"/>
-      <c r="Q47" s="29"/>
-      <c r="R47" s="29"/>
-      <c r="S47" s="29"/>
-      <c r="T47" s="29"/>
-      <c r="U47" s="29"/>
-      <c r="V47" s="29"/>
-      <c r="W47" s="29"/>
-      <c r="X47" s="29"/>
-      <c r="Y47" s="29"/>
-      <c r="Z47" s="29"/>
-      <c r="AA47" s="29"/>
-      <c r="AB47" s="29"/>
-      <c r="AC47" s="29"/>
-      <c r="AD47" s="29"/>
-      <c r="AE47" s="29"/>
-      <c r="AF47" s="29"/>
-      <c r="AG47" s="29"/>
-      <c r="AH47" s="29"/>
-      <c r="AI47" s="29"/>
-      <c r="AJ47" s="29"/>
-      <c r="AK47" s="29"/>
-      <c r="AL47" s="29"/>
-      <c r="AM47" s="29"/>
-      <c r="AN47" s="29"/>
-      <c r="AO47" s="29"/>
-      <c r="AP47" s="29"/>
-      <c r="AQ47" s="29"/>
-      <c r="AR47" s="29"/>
-      <c r="AS47" s="29"/>
-      <c r="AT47" s="29"/>
-      <c r="AU47" s="29"/>
-    </row>
-    <row r="48" spans="1:47">
-      <c r="A48" s="29"/>
-      <c r="B48" s="29"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="29"/>
-      <c r="H48" s="29"/>
-      <c r="I48" s="29"/>
-      <c r="J48" s="29"/>
-      <c r="K48" s="29"/>
-      <c r="L48" s="29"/>
-      <c r="M48" s="29"/>
-      <c r="N48" s="29"/>
-      <c r="O48" s="29"/>
-      <c r="P48" s="29"/>
-      <c r="Q48" s="29"/>
-      <c r="R48" s="29"/>
-      <c r="S48" s="29"/>
-      <c r="T48" s="29"/>
-      <c r="U48" s="29"/>
-      <c r="V48" s="29"/>
-      <c r="W48" s="29"/>
-      <c r="X48" s="29"/>
-      <c r="Y48" s="29"/>
-      <c r="Z48" s="29"/>
-      <c r="AA48" s="29"/>
-      <c r="AB48" s="29"/>
-      <c r="AC48" s="29"/>
-      <c r="AD48" s="29"/>
-      <c r="AE48" s="29"/>
-      <c r="AF48" s="29"/>
-      <c r="AG48" s="29"/>
-      <c r="AH48" s="29"/>
-      <c r="AI48" s="29"/>
-      <c r="AJ48" s="29"/>
-      <c r="AK48" s="29"/>
-      <c r="AL48" s="29"/>
-      <c r="AM48" s="29"/>
-      <c r="AN48" s="29"/>
-      <c r="AO48" s="29"/>
-      <c r="AP48" s="29"/>
-      <c r="AQ48" s="29"/>
-      <c r="AR48" s="29"/>
-      <c r="AS48" s="29"/>
-      <c r="AT48" s="29"/>
-      <c r="AU48" s="29"/>
-    </row>
-    <row r="49" spans="1:47">
-      <c r="A49" s="29"/>
-      <c r="B49" s="29"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="29"/>
-      <c r="G49" s="29"/>
-      <c r="H49" s="29"/>
-      <c r="I49" s="29"/>
-      <c r="J49" s="29"/>
-      <c r="K49" s="29"/>
-      <c r="L49" s="29"/>
-      <c r="M49" s="29"/>
-      <c r="N49" s="29"/>
-      <c r="O49" s="29"/>
-      <c r="P49" s="29"/>
-      <c r="Q49" s="29"/>
-      <c r="R49" s="29"/>
-      <c r="S49" s="29"/>
-      <c r="T49" s="29"/>
-      <c r="U49" s="29"/>
-      <c r="V49" s="29"/>
-      <c r="W49" s="29"/>
-      <c r="X49" s="29"/>
-      <c r="Y49" s="29"/>
-      <c r="Z49" s="29"/>
-      <c r="AA49" s="29"/>
-      <c r="AB49" s="29"/>
-      <c r="AC49" s="29"/>
-      <c r="AD49" s="29"/>
-      <c r="AE49" s="29"/>
-      <c r="AF49" s="29"/>
-      <c r="AG49" s="29"/>
-      <c r="AH49" s="29"/>
-      <c r="AI49" s="29"/>
-      <c r="AJ49" s="29"/>
-      <c r="AK49" s="29"/>
-      <c r="AL49" s="29"/>
-      <c r="AM49" s="29"/>
-      <c r="AN49" s="29"/>
-      <c r="AO49" s="29"/>
-      <c r="AP49" s="29"/>
-      <c r="AQ49" s="29"/>
-      <c r="AR49" s="29"/>
-      <c r="AS49" s="29"/>
-      <c r="AT49" s="29"/>
-      <c r="AU49" s="29"/>
-    </row>
-    <row r="50" spans="1:47">
-      <c r="A50" s="29"/>
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
-      <c r="I50" s="29"/>
-      <c r="J50" s="29"/>
-      <c r="K50" s="29"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="29"/>
-      <c r="N50" s="29"/>
-      <c r="O50" s="29"/>
-      <c r="P50" s="29"/>
-      <c r="Q50" s="29"/>
-      <c r="R50" s="29"/>
-      <c r="S50" s="29"/>
-      <c r="T50" s="29"/>
-      <c r="U50" s="29"/>
-      <c r="V50" s="29"/>
-      <c r="W50" s="29"/>
-      <c r="X50" s="29"/>
-      <c r="Y50" s="29"/>
-      <c r="Z50" s="29"/>
-      <c r="AA50" s="29"/>
-      <c r="AB50" s="29"/>
-      <c r="AC50" s="29"/>
-      <c r="AD50" s="29"/>
-      <c r="AE50" s="29"/>
-      <c r="AF50" s="29"/>
-      <c r="AG50" s="29"/>
-      <c r="AH50" s="29"/>
-      <c r="AI50" s="29"/>
-      <c r="AJ50" s="29"/>
-      <c r="AK50" s="29"/>
-      <c r="AL50" s="29"/>
-      <c r="AM50" s="29"/>
-      <c r="AN50" s="29"/>
-      <c r="AO50" s="29"/>
-      <c r="AP50" s="29"/>
-      <c r="AQ50" s="29"/>
-      <c r="AR50" s="29"/>
-      <c r="AS50" s="29"/>
-      <c r="AT50" s="29"/>
-      <c r="AU50" s="29"/>
-    </row>
-    <row r="51" spans="1:47">
-      <c r="A51" s="29"/>
-      <c r="B51" s="29"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="29"/>
-      <c r="H51" s="29"/>
-      <c r="I51" s="29"/>
-      <c r="J51" s="29"/>
-      <c r="K51" s="29"/>
-      <c r="L51" s="29"/>
-      <c r="M51" s="29"/>
-      <c r="N51" s="29"/>
-      <c r="O51" s="29"/>
-      <c r="P51" s="29"/>
-      <c r="Q51" s="29"/>
-      <c r="R51" s="29"/>
-      <c r="S51" s="29"/>
-      <c r="T51" s="29"/>
-      <c r="U51" s="29"/>
-      <c r="V51" s="29"/>
-      <c r="W51" s="29"/>
-      <c r="X51" s="29"/>
-      <c r="Y51" s="29"/>
-      <c r="Z51" s="29"/>
-      <c r="AA51" s="29"/>
-      <c r="AB51" s="29"/>
-      <c r="AC51" s="29"/>
-      <c r="AD51" s="29"/>
-      <c r="AE51" s="29"/>
-      <c r="AF51" s="29"/>
-      <c r="AG51" s="29"/>
-      <c r="AH51" s="29"/>
-      <c r="AI51" s="29"/>
-      <c r="AJ51" s="29"/>
-      <c r="AK51" s="29"/>
-      <c r="AL51" s="29"/>
-      <c r="AM51" s="29"/>
-      <c r="AN51" s="29"/>
-      <c r="AO51" s="29"/>
-      <c r="AP51" s="29"/>
-      <c r="AQ51" s="29"/>
-      <c r="AR51" s="29"/>
-      <c r="AS51" s="29"/>
-      <c r="AT51" s="29"/>
-      <c r="AU51" s="29"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="66"/>
+      <c r="J26" s="66"/>
+      <c r="K26" s="66"/>
+      <c r="L26" s="66"/>
+    </row>
+    <row r="27" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A27" s="72"/>
+      <c r="B27" s="68"/>
+      <c r="C27" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="D27" s="73"/>
+      <c r="E27" s="94"/>
+      <c r="F27" s="80"/>
+      <c r="G27" s="80"/>
+      <c r="H27" s="66"/>
+      <c r="I27" s="66"/>
+      <c r="J27" s="66"/>
+      <c r="K27" s="66"/>
+      <c r="L27" s="66"/>
+    </row>
+    <row r="28" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A28" s="72"/>
+      <c r="B28" s="68"/>
+      <c r="C28" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="D28" s="73"/>
+      <c r="E28" s="94"/>
+      <c r="F28" s="80"/>
+      <c r="G28" s="80"/>
+      <c r="H28" s="67"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="67"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="67"/>
+    </row>
+    <row r="29" spans="1:12" s="12" customFormat="1" ht="13.2">
+      <c r="A29" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="62" t="s">
+        <v>202</v>
+      </c>
+      <c r="C29" s="63"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
+    </row>
+    <row r="30" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A30" s="72"/>
+      <c r="B30" s="68" t="s">
+        <v>164</v>
+      </c>
+      <c r="C30" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="D30" s="73" t="s">
+        <v>216</v>
+      </c>
+      <c r="E30" s="93" t="s">
+        <v>204</v>
+      </c>
+      <c r="F30" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="G30" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="H30" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="J30" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="K30" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="L30" s="80" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="28" customFormat="1" ht="36" customHeight="1" outlineLevel="1">
+      <c r="A31" s="72"/>
+      <c r="B31" s="68"/>
+      <c r="C31" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="D31" s="73"/>
+      <c r="E31" s="93"/>
+      <c r="F31" s="80"/>
+      <c r="G31" s="80"/>
+      <c r="H31" s="80"/>
+      <c r="I31" s="80"/>
+      <c r="J31" s="80"/>
+      <c r="K31" s="80"/>
+      <c r="L31" s="80"/>
+    </row>
+    <row r="32" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A32" s="72"/>
+      <c r="B32" s="68"/>
+      <c r="C32" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="D32" s="73"/>
+      <c r="E32" s="93"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="80"/>
+      <c r="I32" s="80"/>
+      <c r="J32" s="80"/>
+      <c r="K32" s="80"/>
+      <c r="L32" s="80"/>
+    </row>
+    <row r="33" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A33" s="72"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="D33" s="73"/>
+      <c r="E33" s="93"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="80"/>
+      <c r="H33" s="80"/>
+      <c r="I33" s="80"/>
+      <c r="J33" s="80"/>
+      <c r="K33" s="80"/>
+      <c r="L33" s="80"/>
+    </row>
+    <row r="34" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A34" s="72"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="D34" s="73"/>
+      <c r="E34" s="93"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="80"/>
+      <c r="H34" s="80"/>
+      <c r="I34" s="80"/>
+      <c r="J34" s="80"/>
+      <c r="K34" s="80"/>
+      <c r="L34" s="80"/>
+    </row>
+    <row r="35" spans="1:12" s="12" customFormat="1" ht="13.2">
+      <c r="A35" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="62" t="s">
+        <v>206</v>
+      </c>
+      <c r="C35" s="63"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" s="33"/>
+      <c r="J35" s="33"/>
+      <c r="K35" s="33"/>
+      <c r="L35" s="33"/>
+    </row>
+    <row r="36" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A36" s="72"/>
+      <c r="B36" s="68" t="s">
+        <v>164</v>
+      </c>
+      <c r="C36" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="D36" s="73" t="s">
+        <v>215</v>
+      </c>
+      <c r="E36" s="93" t="s">
+        <v>211</v>
+      </c>
+      <c r="F36" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="H36" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="I36" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="J36" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="K36" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="L36" s="80" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="28" customFormat="1" ht="36" customHeight="1" outlineLevel="1">
+      <c r="A37" s="72"/>
+      <c r="B37" s="68"/>
+      <c r="C37" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="D37" s="73"/>
+      <c r="E37" s="93"/>
+      <c r="F37" s="80"/>
+      <c r="G37" s="80"/>
+      <c r="H37" s="80"/>
+      <c r="I37" s="80"/>
+      <c r="J37" s="80"/>
+      <c r="K37" s="80"/>
+      <c r="L37" s="80"/>
+    </row>
+    <row r="38" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A38" s="72"/>
+      <c r="B38" s="68"/>
+      <c r="C38" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="D38" s="73"/>
+      <c r="E38" s="93"/>
+      <c r="F38" s="80"/>
+      <c r="G38" s="80"/>
+      <c r="H38" s="80"/>
+      <c r="I38" s="80"/>
+      <c r="J38" s="80"/>
+      <c r="K38" s="80"/>
+      <c r="L38" s="80"/>
+    </row>
+    <row r="39" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A39" s="72"/>
+      <c r="B39" s="68"/>
+      <c r="C39" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="D39" s="73"/>
+      <c r="E39" s="93"/>
+      <c r="F39" s="80"/>
+      <c r="G39" s="80"/>
+      <c r="H39" s="80"/>
+      <c r="I39" s="80"/>
+      <c r="J39" s="80"/>
+      <c r="K39" s="80"/>
+      <c r="L39" s="80"/>
+    </row>
+    <row r="40" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A40" s="72"/>
+      <c r="B40" s="68"/>
+      <c r="C40" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="D40" s="73"/>
+      <c r="E40" s="93"/>
+      <c r="F40" s="80"/>
+      <c r="G40" s="80"/>
+      <c r="H40" s="80"/>
+      <c r="I40" s="80"/>
+      <c r="J40" s="80"/>
+      <c r="K40" s="80"/>
+      <c r="L40" s="80"/>
+    </row>
+    <row r="41" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A41" s="72"/>
+      <c r="B41" s="68"/>
+      <c r="C41" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="D41" s="73"/>
+      <c r="E41" s="93"/>
+      <c r="F41" s="80"/>
+      <c r="G41" s="80"/>
+      <c r="H41" s="80"/>
+      <c r="I41" s="80"/>
+      <c r="J41" s="80"/>
+      <c r="K41" s="80"/>
+      <c r="L41" s="80"/>
+    </row>
+    <row r="42" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A42" s="72"/>
+      <c r="B42" s="68"/>
+      <c r="C42" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="D42" s="73"/>
+      <c r="E42" s="93"/>
+      <c r="F42" s="80"/>
+      <c r="G42" s="80"/>
+      <c r="H42" s="80"/>
+      <c r="I42" s="80"/>
+      <c r="J42" s="80"/>
+      <c r="K42" s="80"/>
+      <c r="L42" s="80"/>
+    </row>
+    <row r="43" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A43" s="72"/>
+      <c r="B43" s="68"/>
+      <c r="C43" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="D43" s="73"/>
+      <c r="E43" s="93"/>
+      <c r="F43" s="80"/>
+      <c r="G43" s="80"/>
+      <c r="H43" s="80"/>
+      <c r="I43" s="80"/>
+      <c r="J43" s="80"/>
+      <c r="K43" s="80"/>
+      <c r="L43" s="80"/>
+    </row>
+    <row r="44" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A44" s="72"/>
+      <c r="B44" s="68"/>
+      <c r="C44" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="D44" s="73"/>
+      <c r="E44" s="93"/>
+      <c r="F44" s="80"/>
+      <c r="G44" s="80"/>
+      <c r="H44" s="80"/>
+      <c r="I44" s="80"/>
+      <c r="J44" s="80"/>
+      <c r="K44" s="80"/>
+      <c r="L44" s="80"/>
+    </row>
+    <row r="45" spans="1:12" s="12" customFormat="1" ht="13.2">
+      <c r="A45" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="62" t="s">
+        <v>213</v>
+      </c>
+      <c r="C45" s="63"/>
+      <c r="D45" s="64"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="31"/>
+      <c r="H45" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="33"/>
+      <c r="J45" s="33"/>
+      <c r="K45" s="33"/>
+      <c r="L45" s="33"/>
+    </row>
+    <row r="46" spans="1:12" s="28" customFormat="1" ht="44.4" customHeight="1" outlineLevel="1">
+      <c r="A46" s="72"/>
+      <c r="B46" s="68" t="s">
+        <v>164</v>
+      </c>
+      <c r="C46" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="D46" s="73" t="s">
+        <v>218</v>
+      </c>
+      <c r="E46" s="93"/>
+      <c r="F46" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="G46" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="H46" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="I46" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="J46" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="K46" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="L46" s="80" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" s="28" customFormat="1" ht="44.4" customHeight="1" outlineLevel="1">
+      <c r="A47" s="72"/>
+      <c r="B47" s="68"/>
+      <c r="C47" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="D47" s="73"/>
+      <c r="E47" s="93"/>
+      <c r="F47" s="80"/>
+      <c r="G47" s="80"/>
+      <c r="H47" s="80"/>
+      <c r="I47" s="80"/>
+      <c r="J47" s="80"/>
+      <c r="K47" s="80"/>
+      <c r="L47" s="80"/>
+    </row>
+    <row r="48" spans="1:12" s="28" customFormat="1" ht="44.4" customHeight="1" outlineLevel="1">
+      <c r="A48" s="72"/>
+      <c r="B48" s="68"/>
+      <c r="C48" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="D48" s="73"/>
+      <c r="E48" s="93"/>
+      <c r="F48" s="80"/>
+      <c r="G48" s="80"/>
+      <c r="H48" s="80"/>
+      <c r="I48" s="80"/>
+      <c r="J48" s="80"/>
+      <c r="K48" s="80"/>
+      <c r="L48" s="80"/>
+    </row>
+    <row r="49" spans="1:47" s="28" customFormat="1" ht="44.4" customHeight="1" outlineLevel="1">
+      <c r="A49" s="72"/>
+      <c r="B49" s="68"/>
+      <c r="C49" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="D49" s="73"/>
+      <c r="E49" s="93"/>
+      <c r="F49" s="80"/>
+      <c r="G49" s="80"/>
+      <c r="H49" s="80"/>
+      <c r="I49" s="80"/>
+      <c r="J49" s="80"/>
+      <c r="K49" s="80"/>
+      <c r="L49" s="80"/>
+    </row>
+    <row r="50" spans="1:47" s="28" customFormat="1" ht="44.4" customHeight="1" outlineLevel="1">
+      <c r="A50" s="72"/>
+      <c r="B50" s="68"/>
+      <c r="C50" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="D50" s="73"/>
+      <c r="E50" s="93"/>
+      <c r="F50" s="80"/>
+      <c r="G50" s="80"/>
+      <c r="H50" s="80"/>
+      <c r="I50" s="80"/>
+      <c r="J50" s="80"/>
+      <c r="K50" s="80"/>
+      <c r="L50" s="80"/>
+    </row>
+    <row r="51" spans="1:47" s="28" customFormat="1" ht="44.4" customHeight="1" outlineLevel="1">
+      <c r="A51" s="72"/>
+      <c r="B51" s="68"/>
+      <c r="C51" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="D51" s="73"/>
+      <c r="E51" s="93"/>
+      <c r="F51" s="80"/>
+      <c r="G51" s="80"/>
+      <c r="H51" s="80"/>
+      <c r="I51" s="80"/>
+      <c r="J51" s="80"/>
+      <c r="K51" s="80"/>
+      <c r="L51" s="80"/>
     </row>
     <row r="52" spans="1:47">
       <c r="A52" s="29"/>
@@ -50403,10 +49818,303 @@
       <c r="AT135" s="29"/>
       <c r="AU135" s="29"/>
     </row>
+    <row r="136" spans="1:47">
+      <c r="A136" s="29"/>
+      <c r="B136" s="29"/>
+      <c r="C136" s="29"/>
+      <c r="D136" s="29"/>
+      <c r="E136" s="29"/>
+      <c r="F136" s="29"/>
+      <c r="G136" s="29"/>
+      <c r="H136" s="29"/>
+      <c r="I136" s="29"/>
+      <c r="J136" s="29"/>
+      <c r="K136" s="29"/>
+      <c r="L136" s="29"/>
+      <c r="M136" s="29"/>
+      <c r="N136" s="29"/>
+      <c r="O136" s="29"/>
+      <c r="P136" s="29"/>
+      <c r="Q136" s="29"/>
+      <c r="R136" s="29"/>
+      <c r="S136" s="29"/>
+      <c r="T136" s="29"/>
+      <c r="U136" s="29"/>
+      <c r="V136" s="29"/>
+      <c r="W136" s="29"/>
+      <c r="X136" s="29"/>
+      <c r="Y136" s="29"/>
+      <c r="Z136" s="29"/>
+      <c r="AA136" s="29"/>
+      <c r="AB136" s="29"/>
+      <c r="AC136" s="29"/>
+      <c r="AD136" s="29"/>
+      <c r="AE136" s="29"/>
+      <c r="AF136" s="29"/>
+      <c r="AG136" s="29"/>
+      <c r="AH136" s="29"/>
+      <c r="AI136" s="29"/>
+      <c r="AJ136" s="29"/>
+      <c r="AK136" s="29"/>
+      <c r="AL136" s="29"/>
+      <c r="AM136" s="29"/>
+      <c r="AN136" s="29"/>
+      <c r="AO136" s="29"/>
+      <c r="AP136" s="29"/>
+      <c r="AQ136" s="29"/>
+      <c r="AR136" s="29"/>
+      <c r="AS136" s="29"/>
+      <c r="AT136" s="29"/>
+      <c r="AU136" s="29"/>
+    </row>
+    <row r="137" spans="1:47">
+      <c r="A137" s="29"/>
+      <c r="B137" s="29"/>
+      <c r="C137" s="29"/>
+      <c r="D137" s="29"/>
+      <c r="E137" s="29"/>
+      <c r="F137" s="29"/>
+      <c r="G137" s="29"/>
+      <c r="H137" s="29"/>
+      <c r="I137" s="29"/>
+      <c r="J137" s="29"/>
+      <c r="K137" s="29"/>
+      <c r="L137" s="29"/>
+      <c r="M137" s="29"/>
+      <c r="N137" s="29"/>
+      <c r="O137" s="29"/>
+      <c r="P137" s="29"/>
+      <c r="Q137" s="29"/>
+      <c r="R137" s="29"/>
+      <c r="S137" s="29"/>
+      <c r="T137" s="29"/>
+      <c r="U137" s="29"/>
+      <c r="V137" s="29"/>
+      <c r="W137" s="29"/>
+      <c r="X137" s="29"/>
+      <c r="Y137" s="29"/>
+      <c r="Z137" s="29"/>
+      <c r="AA137" s="29"/>
+      <c r="AB137" s="29"/>
+      <c r="AC137" s="29"/>
+      <c r="AD137" s="29"/>
+      <c r="AE137" s="29"/>
+      <c r="AF137" s="29"/>
+      <c r="AG137" s="29"/>
+      <c r="AH137" s="29"/>
+      <c r="AI137" s="29"/>
+      <c r="AJ137" s="29"/>
+      <c r="AK137" s="29"/>
+      <c r="AL137" s="29"/>
+      <c r="AM137" s="29"/>
+      <c r="AN137" s="29"/>
+      <c r="AO137" s="29"/>
+      <c r="AP137" s="29"/>
+      <c r="AQ137" s="29"/>
+      <c r="AR137" s="29"/>
+      <c r="AS137" s="29"/>
+      <c r="AT137" s="29"/>
+      <c r="AU137" s="29"/>
+    </row>
+    <row r="138" spans="1:47">
+      <c r="A138" s="29"/>
+      <c r="B138" s="29"/>
+      <c r="C138" s="29"/>
+      <c r="D138" s="29"/>
+      <c r="E138" s="29"/>
+      <c r="F138" s="29"/>
+      <c r="G138" s="29"/>
+      <c r="H138" s="29"/>
+      <c r="I138" s="29"/>
+      <c r="J138" s="29"/>
+      <c r="K138" s="29"/>
+      <c r="L138" s="29"/>
+      <c r="M138" s="29"/>
+      <c r="N138" s="29"/>
+      <c r="O138" s="29"/>
+      <c r="P138" s="29"/>
+      <c r="Q138" s="29"/>
+      <c r="R138" s="29"/>
+      <c r="S138" s="29"/>
+      <c r="T138" s="29"/>
+      <c r="U138" s="29"/>
+      <c r="V138" s="29"/>
+      <c r="W138" s="29"/>
+      <c r="X138" s="29"/>
+      <c r="Y138" s="29"/>
+      <c r="Z138" s="29"/>
+      <c r="AA138" s="29"/>
+      <c r="AB138" s="29"/>
+      <c r="AC138" s="29"/>
+      <c r="AD138" s="29"/>
+      <c r="AE138" s="29"/>
+      <c r="AF138" s="29"/>
+      <c r="AG138" s="29"/>
+      <c r="AH138" s="29"/>
+      <c r="AI138" s="29"/>
+      <c r="AJ138" s="29"/>
+      <c r="AK138" s="29"/>
+      <c r="AL138" s="29"/>
+      <c r="AM138" s="29"/>
+      <c r="AN138" s="29"/>
+      <c r="AO138" s="29"/>
+      <c r="AP138" s="29"/>
+      <c r="AQ138" s="29"/>
+      <c r="AR138" s="29"/>
+      <c r="AS138" s="29"/>
+      <c r="AT138" s="29"/>
+      <c r="AU138" s="29"/>
+    </row>
+    <row r="139" spans="1:47">
+      <c r="A139" s="29"/>
+      <c r="B139" s="29"/>
+      <c r="C139" s="29"/>
+      <c r="D139" s="29"/>
+      <c r="E139" s="29"/>
+      <c r="F139" s="29"/>
+      <c r="G139" s="29"/>
+      <c r="H139" s="29"/>
+      <c r="I139" s="29"/>
+      <c r="J139" s="29"/>
+      <c r="K139" s="29"/>
+      <c r="L139" s="29"/>
+      <c r="M139" s="29"/>
+      <c r="N139" s="29"/>
+      <c r="O139" s="29"/>
+      <c r="P139" s="29"/>
+      <c r="Q139" s="29"/>
+      <c r="R139" s="29"/>
+      <c r="S139" s="29"/>
+      <c r="T139" s="29"/>
+      <c r="U139" s="29"/>
+      <c r="V139" s="29"/>
+      <c r="W139" s="29"/>
+      <c r="X139" s="29"/>
+      <c r="Y139" s="29"/>
+      <c r="Z139" s="29"/>
+      <c r="AA139" s="29"/>
+      <c r="AB139" s="29"/>
+      <c r="AC139" s="29"/>
+      <c r="AD139" s="29"/>
+      <c r="AE139" s="29"/>
+      <c r="AF139" s="29"/>
+      <c r="AG139" s="29"/>
+      <c r="AH139" s="29"/>
+      <c r="AI139" s="29"/>
+      <c r="AJ139" s="29"/>
+      <c r="AK139" s="29"/>
+      <c r="AL139" s="29"/>
+      <c r="AM139" s="29"/>
+      <c r="AN139" s="29"/>
+      <c r="AO139" s="29"/>
+      <c r="AP139" s="29"/>
+      <c r="AQ139" s="29"/>
+      <c r="AR139" s="29"/>
+      <c r="AS139" s="29"/>
+      <c r="AT139" s="29"/>
+      <c r="AU139" s="29"/>
+    </row>
+    <row r="140" spans="1:47">
+      <c r="A140" s="29"/>
+      <c r="B140" s="29"/>
+      <c r="C140" s="29"/>
+      <c r="D140" s="29"/>
+      <c r="E140" s="29"/>
+      <c r="F140" s="29"/>
+      <c r="G140" s="29"/>
+      <c r="H140" s="29"/>
+      <c r="I140" s="29"/>
+      <c r="J140" s="29"/>
+      <c r="K140" s="29"/>
+      <c r="L140" s="29"/>
+      <c r="M140" s="29"/>
+      <c r="N140" s="29"/>
+      <c r="O140" s="29"/>
+      <c r="P140" s="29"/>
+      <c r="Q140" s="29"/>
+      <c r="R140" s="29"/>
+      <c r="S140" s="29"/>
+      <c r="T140" s="29"/>
+      <c r="U140" s="29"/>
+      <c r="V140" s="29"/>
+      <c r="W140" s="29"/>
+      <c r="X140" s="29"/>
+      <c r="Y140" s="29"/>
+      <c r="Z140" s="29"/>
+      <c r="AA140" s="29"/>
+      <c r="AB140" s="29"/>
+      <c r="AC140" s="29"/>
+      <c r="AD140" s="29"/>
+      <c r="AE140" s="29"/>
+      <c r="AF140" s="29"/>
+      <c r="AG140" s="29"/>
+      <c r="AH140" s="29"/>
+      <c r="AI140" s="29"/>
+      <c r="AJ140" s="29"/>
+      <c r="AK140" s="29"/>
+      <c r="AL140" s="29"/>
+      <c r="AM140" s="29"/>
+      <c r="AN140" s="29"/>
+      <c r="AO140" s="29"/>
+      <c r="AP140" s="29"/>
+      <c r="AQ140" s="29"/>
+      <c r="AR140" s="29"/>
+      <c r="AS140" s="29"/>
+      <c r="AT140" s="29"/>
+      <c r="AU140" s="29"/>
+    </row>
+    <row r="141" spans="1:47">
+      <c r="A141" s="29"/>
+      <c r="B141" s="29"/>
+      <c r="C141" s="29"/>
+      <c r="D141" s="29"/>
+      <c r="E141" s="29"/>
+      <c r="F141" s="29"/>
+      <c r="G141" s="29"/>
+      <c r="H141" s="29"/>
+      <c r="I141" s="29"/>
+      <c r="J141" s="29"/>
+      <c r="K141" s="29"/>
+      <c r="L141" s="29"/>
+      <c r="M141" s="29"/>
+      <c r="N141" s="29"/>
+      <c r="O141" s="29"/>
+      <c r="P141" s="29"/>
+      <c r="Q141" s="29"/>
+      <c r="R141" s="29"/>
+      <c r="S141" s="29"/>
+      <c r="T141" s="29"/>
+      <c r="U141" s="29"/>
+      <c r="V141" s="29"/>
+      <c r="W141" s="29"/>
+      <c r="X141" s="29"/>
+      <c r="Y141" s="29"/>
+      <c r="Z141" s="29"/>
+      <c r="AA141" s="29"/>
+      <c r="AB141" s="29"/>
+      <c r="AC141" s="29"/>
+      <c r="AD141" s="29"/>
+      <c r="AE141" s="29"/>
+      <c r="AF141" s="29"/>
+      <c r="AG141" s="29"/>
+      <c r="AH141" s="29"/>
+      <c r="AI141" s="29"/>
+      <c r="AJ141" s="29"/>
+      <c r="AK141" s="29"/>
+      <c r="AL141" s="29"/>
+      <c r="AM141" s="29"/>
+      <c r="AN141" s="29"/>
+      <c r="AO141" s="29"/>
+      <c r="AP141" s="29"/>
+      <c r="AQ141" s="29"/>
+      <c r="AR141" s="29"/>
+      <c r="AS141" s="29"/>
+      <c r="AT141" s="29"/>
+      <c r="AU141" s="29"/>
+    </row>
   </sheetData>
   <autoFilter ref="A22:L22" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
-  <mergeCells count="23">
-    <mergeCell ref="H21:L21"/>
+  <mergeCells count="59">
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:C3"/>
@@ -50414,27 +50122,64 @@
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
-    <mergeCell ref="G24:G26"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="K24:K26"/>
-    <mergeCell ref="L24:L26"/>
+    <mergeCell ref="H21:L21"/>
+    <mergeCell ref="L24:L28"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="B30:B34"/>
+    <mergeCell ref="D30:D34"/>
+    <mergeCell ref="F30:F34"/>
+    <mergeCell ref="G30:G34"/>
+    <mergeCell ref="H30:H34"/>
+    <mergeCell ref="I30:I34"/>
+    <mergeCell ref="J30:J34"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E30:E34"/>
+    <mergeCell ref="G24:G28"/>
+    <mergeCell ref="H24:H28"/>
+    <mergeCell ref="I24:I28"/>
+    <mergeCell ref="J24:J28"/>
+    <mergeCell ref="K24:K28"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="D24:D28"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="K30:K34"/>
+    <mergeCell ref="L30:L34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="A36:A44"/>
+    <mergeCell ref="B36:B44"/>
+    <mergeCell ref="D36:D44"/>
+    <mergeCell ref="E36:E44"/>
+    <mergeCell ref="F36:F44"/>
+    <mergeCell ref="G36:G44"/>
+    <mergeCell ref="H36:H44"/>
+    <mergeCell ref="I36:I44"/>
+    <mergeCell ref="J36:J44"/>
+    <mergeCell ref="K36:K44"/>
+    <mergeCell ref="L36:L44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="A46:A51"/>
+    <mergeCell ref="B46:B51"/>
+    <mergeCell ref="D46:D51"/>
+    <mergeCell ref="E46:E51"/>
+    <mergeCell ref="K46:K51"/>
+    <mergeCell ref="L46:L51"/>
+    <mergeCell ref="F46:F51"/>
+    <mergeCell ref="G46:G51"/>
+    <mergeCell ref="H46:H51"/>
+    <mergeCell ref="I46:I51"/>
+    <mergeCell ref="J46:J51"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" sqref="MFX23:MGA26 AMR23:AMU26 SHL23:SHO26 AWN23:AWQ26 MPT23:MPW26 BGJ23:BGM26 VIF23:VII26 BQF23:BQI26 MZP23:MZS26 CAB23:CAE26 SRH23:SRK26 CJX23:CKA26 NJL23:NJO26 CTT23:CTW26 WVP23:WVS26 DDP23:DDS26 NTH23:NTK26 DNL23:DNO26 TBD23:TBG26 DXH23:DXK26 ODD23:ODG26 EHD23:EHG26 VSB23:VSE26 EQZ23:ERC26 OMZ23:ONC26 FAV23:FAY26 TKZ23:TLC26 FKR23:FKU26 OWV23:OWY26 FUN23:FUQ26 JD23:JG26 GEJ23:GEM26 PGR23:PGU26 GOF23:GOI26 TUV23:TUY26 GYB23:GYE26 PQN23:PQQ26 HHX23:HIA26 WBX23:WCA26 HRT23:HRW26 QAJ23:QAM26 IBP23:IBS26 UER23:UEU26 ILL23:ILO26 QKF23:QKI26 IVH23:IVK26 SZ23:TC26 JFD23:JFG26 QUB23:QUE26 JOZ23:JPC26 UON23:UOQ26 JYV23:JYY26 RDX23:REA26 KIR23:KIU26 WLT23:WLW26 KSN23:KSQ26 RNT23:RNW26 LCJ23:LCM26 UYJ23:UYM26 LMF23:LMI26 RXP23:RXS26 LWB23:LWE26 ACV23:ACY26" xr:uid="{F10FE83F-61D8-4140-B18D-7D0CA26FA4EB}">
+    <dataValidation type="list" allowBlank="1" sqref="MFX23:MGA51 AMR23:AMU51 SHL23:SHO51 AWN23:AWQ51 MPT23:MPW51 BGJ23:BGM51 VIF23:VII51 BQF23:BQI51 MZP23:MZS51 CAB23:CAE51 SRH23:SRK51 CJX23:CKA51 NJL23:NJO51 CTT23:CTW51 WVP23:WVS51 DDP23:DDS51 NTH23:NTK51 DNL23:DNO51 TBD23:TBG51 DXH23:DXK51 ODD23:ODG51 EHD23:EHG51 VSB23:VSE51 EQZ23:ERC51 OMZ23:ONC51 FAV23:FAY51 TKZ23:TLC51 FKR23:FKU51 OWV23:OWY51 FUN23:FUQ51 JD23:JG51 GEJ23:GEM51 PGR23:PGU51 GOF23:GOI51 TUV23:TUY51 GYB23:GYE51 PQN23:PQQ51 HHX23:HIA51 WBX23:WCA51 HRT23:HRW51 QAJ23:QAM51 IBP23:IBS51 UER23:UEU51 ILL23:ILO51 QKF23:QKI51 IVH23:IVK51 SZ23:TC51 JFD23:JFG51 QUB23:QUE51 JOZ23:JPC51 UON23:UOQ51 JYV23:JYY51 RDX23:REA51 KIR23:KIU51 WLT23:WLW51 KSN23:KSQ51 RNT23:RNW51 LCJ23:LCM51 UYJ23:UYM51 LMF23:LMI51 RXP23:RXS51 LWB23:LWE51 ACV23:ACY51" xr:uid="{F10FE83F-61D8-4140-B18D-7D0CA26FA4EB}">
       <formula1>$A$14:$A$19</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="H23:L23" xr:uid="{4E16EDCF-1303-49A3-B4E2-32D5BBAC46DF}">
+    <dataValidation type="list" allowBlank="1" sqref="H23:L23 H29:L29 H35:L35 H45:L45" xr:uid="{4E16EDCF-1303-49A3-B4E2-32D5BBAC46DF}">
       <formula1>$B$13:$G$13</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{52397D1C-D727-4879-8F3C-C418CCE9A0FD}">
@@ -50444,6 +50189,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A23 A29 A35 A45" numberStoredAsText="1"/>
+  </ignoredErrors>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update TC002 for AddToCart func
</commit_message>
<xml_diff>
--- a/ZombieClothing Manual TCs_VinhTran.xlsx
+++ b/ZombieClothing Manual TCs_VinhTran.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\REFERENCES\VLU-SENIOR.SEMES1\AUTE\Project Manual TCs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843894E7-B795-4F33-9ACB-00D8452C8F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9459EECD-CB05-4E5B-8358-409717D60278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" firstSheet="4" activeTab="6" xr2:uid="{D5A25300-DCC6-4734-BB7F-F53EA33C6D7D}"/>
   </bookViews>
@@ -740,7 +740,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="229">
   <si>
     <t>Func - Module</t>
   </si>
@@ -1417,13 +1417,7 @@
     <t>Kiểm tra rằng user add to cart thành công khi thêm 1 sản phẩm vào giỏ hàng với số lượng 1</t>
   </si>
   <si>
-    <t>Kiểm tra rằng user add to cart thành công khi thêm 1 sản phẩm vào giỏ hàng với số lượng nhiều hơn 1</t>
-  </si>
-  <si>
     <t>5. Kiểm tra các thông tin có hợp lệ tại trang Giỏ hàng của bạn</t>
-  </si>
-  <si>
-    <t>1&lt;=${toTalProduct}&lt;=100</t>
   </si>
   <si>
     <t>6. Click vào nút Thêm vào giỏ hàng</t>
@@ -1560,6 +1554,42 @@
   </si>
   <si>
     <t>6. Kiểm tra lại các thông tin được hiển thị có hợp lệ khi Xóa sản phẩm khỏi Giỏ hàng</t>
+  </si>
+  <si>
+    <t>2. Hover chuột vào anchor Sản phẩm</t>
+  </si>
+  <si>
+    <t>Kiểm tra rằng user add to cart thành công khi thêm 1 sản phẩm loại nhẫn còn bán vào giỏ hàng với số lượng nhiều hơn 1</t>
+  </si>
+  <si>
+    <t>3. Hover chuột vào anchor Phụ kiện</t>
+  </si>
+  <si>
+    <t>4. Click vào anchor Nhẫn</t>
+  </si>
+  <si>
+    <t>5. Chọn một nhẫn vẫn còn hàng từ danh sách Nhẫn</t>
+  </si>
+  <si>
+    <t>7. Click vào nút Xem giỏ hàng được popped up</t>
+  </si>
+  <si>
+    <t>8. Click vào icon "+" để tăng số lượng nhẫn muốn mua</t>
+  </si>
+  <si>
+    <t>5. Chọn một nhẫn đã hết hàng từ danh sách Nhẫn</t>
+  </si>
+  <si>
+    <t>6. Kiểm tra thông báo hết hàng đã được hiển tị</t>
+  </si>
+  <si>
+    <t>Kiểm tra rằng user add to cart không thành công khi thêm 1 sản phẩm loại nhẫn không còn hàng vào giỏ hàng</t>
+  </si>
+  <si>
+    <t>- Hệ thống navigate user vào trang chi tiết sản phẩm với các elements sau:
++ Một label hiển thị sản phẩm đã Hết hàng
++ Một button hiển thị sản phẩm đã Hết hàng
++ Add to cart không thành công!</t>
   </si>
 </sst>
 </file>
@@ -1866,7 +1896,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2143,6 +2173,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="3" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -44663,10 +44705,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:AU141"/>
+  <dimension ref="A1:AU152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D117" sqref="D117"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" outlineLevelRow="1"/>
@@ -44878,27 +44920,27 @@
         <v>Build1</v>
       </c>
       <c r="B14" s="19">
-        <f t="shared" ref="B14:G14" si="0">COUNTIF($L$23:$L$48468,B13)</f>
+        <f>COUNTIF($L$23:$L$48479,B13)</f>
         <v>0</v>
       </c>
       <c r="C14" s="19">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($L$23:$L$48479,C13)</f>
         <v>0</v>
       </c>
       <c r="D14" s="19">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($L$23:$L$48479,D13)</f>
         <v>0</v>
       </c>
       <c r="E14" s="19">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($L$23:$L$48479,E13)</f>
         <v>0</v>
       </c>
       <c r="F14" s="19">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($L$23:$L$48479,F13)</f>
         <v>0</v>
       </c>
       <c r="G14" s="19">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($L$23:$L$48479,G13)</f>
         <v>0</v>
       </c>
       <c r="H14" s="20"/>
@@ -44913,27 +44955,27 @@
         <v>Build2</v>
       </c>
       <c r="B15" s="19">
-        <f t="shared" ref="B15:G15" si="1">COUNTIF($K$23:$K$48468,B13)</f>
+        <f>COUNTIF($K$23:$K$48479,B13)</f>
         <v>0</v>
       </c>
       <c r="C15" s="19">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($K$23:$K$48479,C13)</f>
         <v>0</v>
       </c>
       <c r="D15" s="19">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($K$23:$K$48479,D13)</f>
         <v>0</v>
       </c>
       <c r="E15" s="19">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($K$23:$K$48479,E13)</f>
         <v>0</v>
       </c>
       <c r="F15" s="19">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($K$23:$K$48479,F13)</f>
         <v>0</v>
       </c>
       <c r="G15" s="19">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($K$23:$K$48479,G13)</f>
         <v>0</v>
       </c>
       <c r="H15" s="20"/>
@@ -44948,27 +44990,27 @@
         <v>Build3</v>
       </c>
       <c r="B16" s="19">
-        <f t="shared" ref="B16:G16" si="2">COUNTIF($J$23:$J$48468,B13)</f>
+        <f>COUNTIF($J$23:$J$48479,B13)</f>
         <v>0</v>
       </c>
       <c r="C16" s="19">
-        <f t="shared" si="2"/>
+        <f>COUNTIF($J$23:$J$48479,C13)</f>
         <v>0</v>
       </c>
       <c r="D16" s="19">
-        <f t="shared" si="2"/>
+        <f>COUNTIF($J$23:$J$48479,D13)</f>
         <v>0</v>
       </c>
       <c r="E16" s="19">
-        <f t="shared" si="2"/>
+        <f>COUNTIF($J$23:$J$48479,E13)</f>
         <v>0</v>
       </c>
       <c r="F16" s="19">
-        <f t="shared" si="2"/>
+        <f>COUNTIF($J$23:$J$48479,F13)</f>
         <v>0</v>
       </c>
       <c r="G16" s="19">
-        <f t="shared" si="2"/>
+        <f>COUNTIF($J$23:$J$48479,G13)</f>
         <v>0</v>
       </c>
       <c r="H16" s="20"/>
@@ -44983,27 +45025,27 @@
         <v>Build4</v>
       </c>
       <c r="B17" s="19">
-        <f>COUNTIF($I$23:$I$48468,B13)</f>
+        <f>COUNTIF($I$23:$I$48479,B13)</f>
         <v>0</v>
       </c>
       <c r="C17" s="19">
-        <f>COUNTIF($I$23:$I$48468,C16)</f>
+        <f>COUNTIF($I$23:$I$48479,C16)</f>
         <v>0</v>
       </c>
       <c r="D17" s="19">
-        <f>COUNTIF($I$23:$I$48468,D13)</f>
+        <f>COUNTIF($I$23:$I$48479,D13)</f>
         <v>0</v>
       </c>
       <c r="E17" s="19">
-        <f>COUNTIF($I$23:$I$48468,E13)</f>
+        <f>COUNTIF($I$23:$I$48479,E13)</f>
         <v>0</v>
       </c>
       <c r="F17" s="19">
-        <f>COUNTIF($I$23:$I$48468,F13)</f>
+        <f>COUNTIF($I$23:$I$48479,F13)</f>
         <v>0</v>
       </c>
       <c r="G17" s="19">
-        <f>COUNTIF($I$23:$I$48468,G13)</f>
+        <f>COUNTIF($I$23:$I$48479,G13)</f>
         <v>0</v>
       </c>
       <c r="H17" s="20"/>
@@ -45018,27 +45060,27 @@
         <v>Build5</v>
       </c>
       <c r="B18" s="19">
-        <f t="shared" ref="B18:G18" si="3">COUNTIF($H$23:$H$48468,B13)</f>
+        <f>COUNTIF($H$23:$H$48479,B13)</f>
         <v>0</v>
       </c>
       <c r="C18" s="19">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($H$23:$H$48479,C13)</f>
         <v>0</v>
       </c>
       <c r="D18" s="19">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($H$23:$H$48479,D13)</f>
         <v>0</v>
       </c>
       <c r="E18" s="19">
-        <f t="shared" si="3"/>
-        <v>4</v>
+        <f>COUNTIF($H$23:$H$48479,E13)</f>
+        <v>5</v>
       </c>
       <c r="F18" s="19">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($H$23:$H$48479,F13)</f>
         <v>0</v>
       </c>
       <c r="G18" s="19">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($H$23:$H$48479,G13)</f>
         <v>0</v>
       </c>
       <c r="H18" s="20"/>
@@ -45052,27 +45094,27 @@
         <v>15</v>
       </c>
       <c r="B19" s="22">
-        <f t="shared" ref="B19:G19" si="4">SUM(B14:B18)</f>
+        <f t="shared" ref="B19:G19" si="0">SUM(B14:B18)</f>
         <v>0</v>
       </c>
       <c r="C19" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D19" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E19" s="22">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="F19" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G19" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H19" s="20"/>
@@ -45175,7 +45217,7 @@
         <v>163</v>
       </c>
       <c r="D24" s="73" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E24" s="94"/>
       <c r="F24" s="80" t="s">
@@ -45252,7 +45294,7 @@
       <c r="A28" s="72"/>
       <c r="B28" s="68"/>
       <c r="C28" s="27" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D28" s="73"/>
       <c r="E28" s="94"/>
@@ -45269,7 +45311,7 @@
         <v>85</v>
       </c>
       <c r="B29" s="62" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="C29" s="63"/>
       <c r="D29" s="64"/>
@@ -45293,10 +45335,10 @@
         <v>163</v>
       </c>
       <c r="D30" s="73" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E30" s="93" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="F30" s="80" t="s">
         <v>28</v>
@@ -45324,7 +45366,7 @@
       <c r="A31" s="72"/>
       <c r="B31" s="68"/>
       <c r="C31" s="27" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="D31" s="73"/>
       <c r="E31" s="93"/>
@@ -45336,11 +45378,11 @@
       <c r="K31" s="80"/>
       <c r="L31" s="80"/>
     </row>
-    <row r="32" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+    <row r="32" spans="1:12" s="28" customFormat="1" ht="36" customHeight="1" outlineLevel="1">
       <c r="A32" s="72"/>
       <c r="B32" s="68"/>
       <c r="C32" s="27" t="s">
-        <v>199</v>
+        <v>220</v>
       </c>
       <c r="D32" s="73"/>
       <c r="E32" s="93"/>
@@ -45352,11 +45394,11 @@
       <c r="K32" s="80"/>
       <c r="L32" s="80"/>
     </row>
-    <row r="33" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+    <row r="33" spans="1:12" s="28" customFormat="1" ht="36" customHeight="1" outlineLevel="1">
       <c r="A33" s="72"/>
       <c r="B33" s="68"/>
       <c r="C33" s="27" t="s">
-        <v>200</v>
+        <v>221</v>
       </c>
       <c r="D33" s="73"/>
       <c r="E33" s="93"/>
@@ -45368,11 +45410,11 @@
       <c r="K33" s="80"/>
       <c r="L33" s="80"/>
     </row>
-    <row r="34" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+    <row r="34" spans="1:12" s="28" customFormat="1" ht="36" customHeight="1" outlineLevel="1">
       <c r="A34" s="72"/>
       <c r="B34" s="68"/>
       <c r="C34" s="27" t="s">
-        <v>203</v>
+        <v>222</v>
       </c>
       <c r="D34" s="73"/>
       <c r="E34" s="93"/>
@@ -45384,67 +45426,43 @@
       <c r="K34" s="80"/>
       <c r="L34" s="80"/>
     </row>
-    <row r="35" spans="1:12" s="12" customFormat="1" ht="13.2">
-      <c r="A35" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" s="62" t="s">
-        <v>206</v>
-      </c>
-      <c r="C35" s="63"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="I35" s="33"/>
-      <c r="J35" s="33"/>
-      <c r="K35" s="33"/>
-      <c r="L35" s="33"/>
+    <row r="35" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A35" s="72"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="D35" s="73"/>
+      <c r="E35" s="93"/>
+      <c r="F35" s="80"/>
+      <c r="G35" s="80"/>
+      <c r="H35" s="80"/>
+      <c r="I35" s="80"/>
+      <c r="J35" s="80"/>
+      <c r="K35" s="80"/>
+      <c r="L35" s="80"/>
     </row>
     <row r="36" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
       <c r="A36" s="72"/>
-      <c r="B36" s="68" t="s">
-        <v>164</v>
-      </c>
-      <c r="C36" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="D36" s="73" t="s">
-        <v>215</v>
-      </c>
-      <c r="E36" s="93" t="s">
-        <v>211</v>
-      </c>
-      <c r="F36" s="80" t="s">
-        <v>28</v>
-      </c>
-      <c r="G36" s="80" t="s">
-        <v>28</v>
-      </c>
-      <c r="H36" s="80" t="s">
-        <v>28</v>
-      </c>
-      <c r="I36" s="80" t="s">
-        <v>28</v>
-      </c>
-      <c r="J36" s="80" t="s">
-        <v>28</v>
-      </c>
-      <c r="K36" s="80" t="s">
-        <v>28</v>
-      </c>
-      <c r="L36" s="80" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" s="28" customFormat="1" ht="36" customHeight="1" outlineLevel="1">
+      <c r="B36" s="68"/>
+      <c r="C36" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="D36" s="73"/>
+      <c r="E36" s="93"/>
+      <c r="F36" s="80"/>
+      <c r="G36" s="80"/>
+      <c r="H36" s="80"/>
+      <c r="I36" s="80"/>
+      <c r="J36" s="80"/>
+      <c r="K36" s="80"/>
+      <c r="L36" s="80"/>
+    </row>
+    <row r="37" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
       <c r="A37" s="72"/>
       <c r="B37" s="68"/>
       <c r="C37" s="27" t="s">
-        <v>198</v>
+        <v>224</v>
       </c>
       <c r="D37" s="73"/>
       <c r="E37" s="93"/>
@@ -45460,7 +45478,7 @@
       <c r="A38" s="72"/>
       <c r="B38" s="68"/>
       <c r="C38" s="27" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="D38" s="73"/>
       <c r="E38" s="93"/>
@@ -45472,177 +45490,201 @@
       <c r="K38" s="80"/>
       <c r="L38" s="80"/>
     </row>
-    <row r="39" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
-      <c r="A39" s="72"/>
-      <c r="B39" s="68"/>
-      <c r="C39" s="27" t="s">
-        <v>212</v>
-      </c>
-      <c r="D39" s="73"/>
-      <c r="E39" s="93"/>
-      <c r="F39" s="80"/>
-      <c r="G39" s="80"/>
-      <c r="H39" s="80"/>
-      <c r="I39" s="80"/>
-      <c r="J39" s="80"/>
-      <c r="K39" s="80"/>
-      <c r="L39" s="80"/>
+    <row r="39" spans="1:12" s="12" customFormat="1" ht="13.2">
+      <c r="A39" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" s="62" t="s">
+        <v>227</v>
+      </c>
+      <c r="C39" s="63"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="33"/>
     </row>
     <row r="40" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
-      <c r="A40" s="72"/>
-      <c r="B40" s="68"/>
-      <c r="C40" s="27" t="s">
-        <v>208</v>
-      </c>
-      <c r="D40" s="73"/>
-      <c r="E40" s="93"/>
-      <c r="F40" s="80"/>
-      <c r="G40" s="80"/>
-      <c r="H40" s="80"/>
-      <c r="I40" s="80"/>
-      <c r="J40" s="80"/>
-      <c r="K40" s="80"/>
-      <c r="L40" s="80"/>
-    </row>
-    <row r="41" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
-      <c r="A41" s="72"/>
-      <c r="B41" s="68"/>
+      <c r="A40" s="49"/>
+      <c r="B40" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="C40" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="D40" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="E40" s="95"/>
+      <c r="F40" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="H40" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="I40" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="J40" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="K40" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="L40" s="65" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="28" customFormat="1" ht="36" customHeight="1" outlineLevel="1">
+      <c r="A41" s="50"/>
+      <c r="B41" s="53"/>
       <c r="C41" s="27" t="s">
-        <v>205</v>
-      </c>
-      <c r="D41" s="73"/>
-      <c r="E41" s="93"/>
-      <c r="F41" s="80"/>
-      <c r="G41" s="80"/>
-      <c r="H41" s="80"/>
-      <c r="I41" s="80"/>
-      <c r="J41" s="80"/>
-      <c r="K41" s="80"/>
-      <c r="L41" s="80"/>
-    </row>
-    <row r="42" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
-      <c r="A42" s="72"/>
-      <c r="B42" s="68"/>
+        <v>218</v>
+      </c>
+      <c r="D41" s="56"/>
+      <c r="E41" s="96"/>
+      <c r="F41" s="66"/>
+      <c r="G41" s="66"/>
+      <c r="H41" s="66"/>
+      <c r="I41" s="66"/>
+      <c r="J41" s="66"/>
+      <c r="K41" s="66"/>
+      <c r="L41" s="66"/>
+    </row>
+    <row r="42" spans="1:12" s="28" customFormat="1" ht="36" customHeight="1" outlineLevel="1">
+      <c r="A42" s="50"/>
+      <c r="B42" s="53"/>
       <c r="C42" s="27" t="s">
-        <v>207</v>
-      </c>
-      <c r="D42" s="73"/>
-      <c r="E42" s="93"/>
-      <c r="F42" s="80"/>
-      <c r="G42" s="80"/>
-      <c r="H42" s="80"/>
-      <c r="I42" s="80"/>
-      <c r="J42" s="80"/>
-      <c r="K42" s="80"/>
-      <c r="L42" s="80"/>
-    </row>
-    <row r="43" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
-      <c r="A43" s="72"/>
-      <c r="B43" s="68"/>
+        <v>220</v>
+      </c>
+      <c r="D42" s="56"/>
+      <c r="E42" s="96"/>
+      <c r="F42" s="66"/>
+      <c r="G42" s="66"/>
+      <c r="H42" s="66"/>
+      <c r="I42" s="66"/>
+      <c r="J42" s="66"/>
+      <c r="K42" s="66"/>
+      <c r="L42" s="66"/>
+    </row>
+    <row r="43" spans="1:12" s="28" customFormat="1" ht="36" customHeight="1" outlineLevel="1">
+      <c r="A43" s="50"/>
+      <c r="B43" s="53"/>
       <c r="C43" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="D43" s="56"/>
+      <c r="E43" s="96"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="66"/>
+      <c r="H43" s="66"/>
+      <c r="I43" s="66"/>
+      <c r="J43" s="66"/>
+      <c r="K43" s="66"/>
+      <c r="L43" s="66"/>
+    </row>
+    <row r="44" spans="1:12" s="28" customFormat="1" ht="36" customHeight="1" outlineLevel="1">
+      <c r="A44" s="50"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="D44" s="56"/>
+      <c r="E44" s="96"/>
+      <c r="F44" s="66"/>
+      <c r="G44" s="66"/>
+      <c r="H44" s="66"/>
+      <c r="I44" s="66"/>
+      <c r="J44" s="66"/>
+      <c r="K44" s="66"/>
+      <c r="L44" s="66"/>
+    </row>
+    <row r="45" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A45" s="51"/>
+      <c r="B45" s="54"/>
+      <c r="C45" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="D45" s="98"/>
+      <c r="E45" s="97"/>
+      <c r="F45" s="67"/>
+      <c r="G45" s="67"/>
+      <c r="H45" s="67"/>
+      <c r="I45" s="67"/>
+      <c r="J45" s="67"/>
+      <c r="K45" s="67"/>
+      <c r="L45" s="67"/>
+    </row>
+    <row r="46" spans="1:12" s="12" customFormat="1" ht="13.2">
+      <c r="A46" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46" s="62" t="s">
+        <v>204</v>
+      </c>
+      <c r="C46" s="63"/>
+      <c r="D46" s="64"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="31"/>
+      <c r="H46" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" s="33"/>
+      <c r="J46" s="33"/>
+      <c r="K46" s="33"/>
+      <c r="L46" s="33"/>
+    </row>
+    <row r="47" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A47" s="72"/>
+      <c r="B47" s="68" t="s">
+        <v>164</v>
+      </c>
+      <c r="C47" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="D47" s="73" t="s">
+        <v>213</v>
+      </c>
+      <c r="E47" s="93" t="s">
         <v>209</v>
       </c>
-      <c r="D43" s="73"/>
-      <c r="E43" s="93"/>
-      <c r="F43" s="80"/>
-      <c r="G43" s="80"/>
-      <c r="H43" s="80"/>
-      <c r="I43" s="80"/>
-      <c r="J43" s="80"/>
-      <c r="K43" s="80"/>
-      <c r="L43" s="80"/>
-    </row>
-    <row r="44" spans="1:12" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
-      <c r="A44" s="72"/>
-      <c r="B44" s="68"/>
-      <c r="C44" s="27" t="s">
-        <v>210</v>
-      </c>
-      <c r="D44" s="73"/>
-      <c r="E44" s="93"/>
-      <c r="F44" s="80"/>
-      <c r="G44" s="80"/>
-      <c r="H44" s="80"/>
-      <c r="I44" s="80"/>
-      <c r="J44" s="80"/>
-      <c r="K44" s="80"/>
-      <c r="L44" s="80"/>
-    </row>
-    <row r="45" spans="1:12" s="12" customFormat="1" ht="13.2">
-      <c r="A45" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="B45" s="62" t="s">
-        <v>213</v>
-      </c>
-      <c r="C45" s="63"/>
-      <c r="D45" s="64"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="I45" s="33"/>
-      <c r="J45" s="33"/>
-      <c r="K45" s="33"/>
-      <c r="L45" s="33"/>
-    </row>
-    <row r="46" spans="1:12" s="28" customFormat="1" ht="44.4" customHeight="1" outlineLevel="1">
-      <c r="A46" s="72"/>
-      <c r="B46" s="68" t="s">
-        <v>164</v>
-      </c>
-      <c r="C46" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="D46" s="73" t="s">
-        <v>218</v>
-      </c>
-      <c r="E46" s="93"/>
-      <c r="F46" s="80" t="s">
+      <c r="F47" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="G46" s="80" t="s">
+      <c r="G47" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="H46" s="80" t="s">
+      <c r="H47" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="I46" s="80" t="s">
+      <c r="I47" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="J46" s="80" t="s">
+      <c r="J47" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="K46" s="80" t="s">
+      <c r="K47" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="L46" s="80" t="s">
+      <c r="L47" s="80" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="28" customFormat="1" ht="44.4" customHeight="1" outlineLevel="1">
-      <c r="A47" s="72"/>
-      <c r="B47" s="68"/>
-      <c r="C47" s="27" t="s">
-        <v>198</v>
-      </c>
-      <c r="D47" s="73"/>
-      <c r="E47" s="93"/>
-      <c r="F47" s="80"/>
-      <c r="G47" s="80"/>
-      <c r="H47" s="80"/>
-      <c r="I47" s="80"/>
-      <c r="J47" s="80"/>
-      <c r="K47" s="80"/>
-      <c r="L47" s="80"/>
-    </row>
-    <row r="48" spans="1:12" s="28" customFormat="1" ht="44.4" customHeight="1" outlineLevel="1">
+    <row r="48" spans="1:12" s="28" customFormat="1" ht="36" customHeight="1" outlineLevel="1">
       <c r="A48" s="72"/>
       <c r="B48" s="68"/>
       <c r="C48" s="27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D48" s="73"/>
       <c r="E48" s="93"/>
@@ -45654,11 +45696,11 @@
       <c r="K48" s="80"/>
       <c r="L48" s="80"/>
     </row>
-    <row r="49" spans="1:47" s="28" customFormat="1" ht="44.4" customHeight="1" outlineLevel="1">
+    <row r="49" spans="1:47" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
       <c r="A49" s="72"/>
       <c r="B49" s="68"/>
       <c r="C49" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D49" s="73"/>
       <c r="E49" s="93"/>
@@ -45670,11 +45712,11 @@
       <c r="K49" s="80"/>
       <c r="L49" s="80"/>
     </row>
-    <row r="50" spans="1:47" s="28" customFormat="1" ht="44.4" customHeight="1" outlineLevel="1">
+    <row r="50" spans="1:47" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
       <c r="A50" s="72"/>
       <c r="B50" s="68"/>
       <c r="C50" s="27" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D50" s="73"/>
       <c r="E50" s="93"/>
@@ -45686,11 +45728,11 @@
       <c r="K50" s="80"/>
       <c r="L50" s="80"/>
     </row>
-    <row r="51" spans="1:47" s="28" customFormat="1" ht="44.4" customHeight="1" outlineLevel="1">
+    <row r="51" spans="1:47" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
       <c r="A51" s="72"/>
       <c r="B51" s="68"/>
       <c r="C51" s="27" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="D51" s="73"/>
       <c r="E51" s="93"/>
@@ -45702,544 +45744,203 @@
       <c r="K51" s="80"/>
       <c r="L51" s="80"/>
     </row>
-    <row r="52" spans="1:47">
-      <c r="A52" s="29"/>
-      <c r="B52" s="29"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
-      <c r="G52" s="29"/>
-      <c r="H52" s="29"/>
-      <c r="I52" s="29"/>
-      <c r="J52" s="29"/>
-      <c r="K52" s="29"/>
-      <c r="L52" s="29"/>
-      <c r="M52" s="29"/>
-      <c r="N52" s="29"/>
-      <c r="O52" s="29"/>
-      <c r="P52" s="29"/>
-      <c r="Q52" s="29"/>
-      <c r="R52" s="29"/>
-      <c r="S52" s="29"/>
-      <c r="T52" s="29"/>
-      <c r="U52" s="29"/>
-      <c r="V52" s="29"/>
-      <c r="W52" s="29"/>
-      <c r="X52" s="29"/>
-      <c r="Y52" s="29"/>
-      <c r="Z52" s="29"/>
-      <c r="AA52" s="29"/>
-      <c r="AB52" s="29"/>
-      <c r="AC52" s="29"/>
-      <c r="AD52" s="29"/>
-      <c r="AE52" s="29"/>
-      <c r="AF52" s="29"/>
-      <c r="AG52" s="29"/>
-      <c r="AH52" s="29"/>
-      <c r="AI52" s="29"/>
-      <c r="AJ52" s="29"/>
-      <c r="AK52" s="29"/>
-      <c r="AL52" s="29"/>
-      <c r="AM52" s="29"/>
-      <c r="AN52" s="29"/>
-      <c r="AO52" s="29"/>
-      <c r="AP52" s="29"/>
-      <c r="AQ52" s="29"/>
-      <c r="AR52" s="29"/>
-      <c r="AS52" s="29"/>
-      <c r="AT52" s="29"/>
-      <c r="AU52" s="29"/>
-    </row>
-    <row r="53" spans="1:47">
-      <c r="A53" s="29"/>
-      <c r="B53" s="29"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="29"/>
-      <c r="H53" s="29"/>
-      <c r="I53" s="29"/>
-      <c r="J53" s="29"/>
-      <c r="K53" s="29"/>
-      <c r="L53" s="29"/>
-      <c r="M53" s="29"/>
-      <c r="N53" s="29"/>
-      <c r="O53" s="29"/>
-      <c r="P53" s="29"/>
-      <c r="Q53" s="29"/>
-      <c r="R53" s="29"/>
-      <c r="S53" s="29"/>
-      <c r="T53" s="29"/>
-      <c r="U53" s="29"/>
-      <c r="V53" s="29"/>
-      <c r="W53" s="29"/>
-      <c r="X53" s="29"/>
-      <c r="Y53" s="29"/>
-      <c r="Z53" s="29"/>
-      <c r="AA53" s="29"/>
-      <c r="AB53" s="29"/>
-      <c r="AC53" s="29"/>
-      <c r="AD53" s="29"/>
-      <c r="AE53" s="29"/>
-      <c r="AF53" s="29"/>
-      <c r="AG53" s="29"/>
-      <c r="AH53" s="29"/>
-      <c r="AI53" s="29"/>
-      <c r="AJ53" s="29"/>
-      <c r="AK53" s="29"/>
-      <c r="AL53" s="29"/>
-      <c r="AM53" s="29"/>
-      <c r="AN53" s="29"/>
-      <c r="AO53" s="29"/>
-      <c r="AP53" s="29"/>
-      <c r="AQ53" s="29"/>
-      <c r="AR53" s="29"/>
-      <c r="AS53" s="29"/>
-      <c r="AT53" s="29"/>
-      <c r="AU53" s="29"/>
-    </row>
-    <row r="54" spans="1:47">
-      <c r="A54" s="29"/>
-      <c r="B54" s="29"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="29"/>
-      <c r="H54" s="29"/>
-      <c r="I54" s="29"/>
-      <c r="J54" s="29"/>
-      <c r="K54" s="29"/>
-      <c r="L54" s="29"/>
-      <c r="M54" s="29"/>
-      <c r="N54" s="29"/>
-      <c r="O54" s="29"/>
-      <c r="P54" s="29"/>
-      <c r="Q54" s="29"/>
-      <c r="R54" s="29"/>
-      <c r="S54" s="29"/>
-      <c r="T54" s="29"/>
-      <c r="U54" s="29"/>
-      <c r="V54" s="29"/>
-      <c r="W54" s="29"/>
-      <c r="X54" s="29"/>
-      <c r="Y54" s="29"/>
-      <c r="Z54" s="29"/>
-      <c r="AA54" s="29"/>
-      <c r="AB54" s="29"/>
-      <c r="AC54" s="29"/>
-      <c r="AD54" s="29"/>
-      <c r="AE54" s="29"/>
-      <c r="AF54" s="29"/>
-      <c r="AG54" s="29"/>
-      <c r="AH54" s="29"/>
-      <c r="AI54" s="29"/>
-      <c r="AJ54" s="29"/>
-      <c r="AK54" s="29"/>
-      <c r="AL54" s="29"/>
-      <c r="AM54" s="29"/>
-      <c r="AN54" s="29"/>
-      <c r="AO54" s="29"/>
-      <c r="AP54" s="29"/>
-      <c r="AQ54" s="29"/>
-      <c r="AR54" s="29"/>
-      <c r="AS54" s="29"/>
-      <c r="AT54" s="29"/>
-      <c r="AU54" s="29"/>
-    </row>
-    <row r="55" spans="1:47">
-      <c r="A55" s="29"/>
-      <c r="B55" s="29"/>
-      <c r="C55" s="29"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="29"/>
-      <c r="F55" s="29"/>
-      <c r="G55" s="29"/>
-      <c r="H55" s="29"/>
-      <c r="I55" s="29"/>
-      <c r="J55" s="29"/>
-      <c r="K55" s="29"/>
-      <c r="L55" s="29"/>
-      <c r="M55" s="29"/>
-      <c r="N55" s="29"/>
-      <c r="O55" s="29"/>
-      <c r="P55" s="29"/>
-      <c r="Q55" s="29"/>
-      <c r="R55" s="29"/>
-      <c r="S55" s="29"/>
-      <c r="T55" s="29"/>
-      <c r="U55" s="29"/>
-      <c r="V55" s="29"/>
-      <c r="W55" s="29"/>
-      <c r="X55" s="29"/>
-      <c r="Y55" s="29"/>
-      <c r="Z55" s="29"/>
-      <c r="AA55" s="29"/>
-      <c r="AB55" s="29"/>
-      <c r="AC55" s="29"/>
-      <c r="AD55" s="29"/>
-      <c r="AE55" s="29"/>
-      <c r="AF55" s="29"/>
-      <c r="AG55" s="29"/>
-      <c r="AH55" s="29"/>
-      <c r="AI55" s="29"/>
-      <c r="AJ55" s="29"/>
-      <c r="AK55" s="29"/>
-      <c r="AL55" s="29"/>
-      <c r="AM55" s="29"/>
-      <c r="AN55" s="29"/>
-      <c r="AO55" s="29"/>
-      <c r="AP55" s="29"/>
-      <c r="AQ55" s="29"/>
-      <c r="AR55" s="29"/>
-      <c r="AS55" s="29"/>
-      <c r="AT55" s="29"/>
-      <c r="AU55" s="29"/>
-    </row>
-    <row r="56" spans="1:47">
-      <c r="A56" s="29"/>
-      <c r="B56" s="29"/>
-      <c r="C56" s="29"/>
-      <c r="D56" s="29"/>
-      <c r="E56" s="29"/>
-      <c r="F56" s="29"/>
-      <c r="G56" s="29"/>
-      <c r="H56" s="29"/>
-      <c r="I56" s="29"/>
-      <c r="J56" s="29"/>
-      <c r="K56" s="29"/>
-      <c r="L56" s="29"/>
-      <c r="M56" s="29"/>
-      <c r="N56" s="29"/>
-      <c r="O56" s="29"/>
-      <c r="P56" s="29"/>
-      <c r="Q56" s="29"/>
-      <c r="R56" s="29"/>
-      <c r="S56" s="29"/>
-      <c r="T56" s="29"/>
-      <c r="U56" s="29"/>
-      <c r="V56" s="29"/>
-      <c r="W56" s="29"/>
-      <c r="X56" s="29"/>
-      <c r="Y56" s="29"/>
-      <c r="Z56" s="29"/>
-      <c r="AA56" s="29"/>
-      <c r="AB56" s="29"/>
-      <c r="AC56" s="29"/>
-      <c r="AD56" s="29"/>
-      <c r="AE56" s="29"/>
-      <c r="AF56" s="29"/>
-      <c r="AG56" s="29"/>
-      <c r="AH56" s="29"/>
-      <c r="AI56" s="29"/>
-      <c r="AJ56" s="29"/>
-      <c r="AK56" s="29"/>
-      <c r="AL56" s="29"/>
-      <c r="AM56" s="29"/>
-      <c r="AN56" s="29"/>
-      <c r="AO56" s="29"/>
-      <c r="AP56" s="29"/>
-      <c r="AQ56" s="29"/>
-      <c r="AR56" s="29"/>
-      <c r="AS56" s="29"/>
-      <c r="AT56" s="29"/>
-      <c r="AU56" s="29"/>
-    </row>
-    <row r="57" spans="1:47">
-      <c r="A57" s="29"/>
-      <c r="B57" s="29"/>
-      <c r="C57" s="29"/>
-      <c r="D57" s="29"/>
-      <c r="E57" s="29"/>
-      <c r="F57" s="29"/>
-      <c r="G57" s="29"/>
-      <c r="H57" s="29"/>
-      <c r="I57" s="29"/>
-      <c r="J57" s="29"/>
-      <c r="K57" s="29"/>
-      <c r="L57" s="29"/>
-      <c r="M57" s="29"/>
-      <c r="N57" s="29"/>
-      <c r="O57" s="29"/>
-      <c r="P57" s="29"/>
-      <c r="Q57" s="29"/>
-      <c r="R57" s="29"/>
-      <c r="S57" s="29"/>
-      <c r="T57" s="29"/>
-      <c r="U57" s="29"/>
-      <c r="V57" s="29"/>
-      <c r="W57" s="29"/>
-      <c r="X57" s="29"/>
-      <c r="Y57" s="29"/>
-      <c r="Z57" s="29"/>
-      <c r="AA57" s="29"/>
-      <c r="AB57" s="29"/>
-      <c r="AC57" s="29"/>
-      <c r="AD57" s="29"/>
-      <c r="AE57" s="29"/>
-      <c r="AF57" s="29"/>
-      <c r="AG57" s="29"/>
-      <c r="AH57" s="29"/>
-      <c r="AI57" s="29"/>
-      <c r="AJ57" s="29"/>
-      <c r="AK57" s="29"/>
-      <c r="AL57" s="29"/>
-      <c r="AM57" s="29"/>
-      <c r="AN57" s="29"/>
-      <c r="AO57" s="29"/>
-      <c r="AP57" s="29"/>
-      <c r="AQ57" s="29"/>
-      <c r="AR57" s="29"/>
-      <c r="AS57" s="29"/>
-      <c r="AT57" s="29"/>
-      <c r="AU57" s="29"/>
-    </row>
-    <row r="58" spans="1:47">
-      <c r="A58" s="29"/>
-      <c r="B58" s="29"/>
-      <c r="C58" s="29"/>
-      <c r="D58" s="29"/>
-      <c r="E58" s="29"/>
-      <c r="F58" s="29"/>
-      <c r="G58" s="29"/>
-      <c r="H58" s="29"/>
-      <c r="I58" s="29"/>
-      <c r="J58" s="29"/>
-      <c r="K58" s="29"/>
-      <c r="L58" s="29"/>
-      <c r="M58" s="29"/>
-      <c r="N58" s="29"/>
-      <c r="O58" s="29"/>
-      <c r="P58" s="29"/>
-      <c r="Q58" s="29"/>
-      <c r="R58" s="29"/>
-      <c r="S58" s="29"/>
-      <c r="T58" s="29"/>
-      <c r="U58" s="29"/>
-      <c r="V58" s="29"/>
-      <c r="W58" s="29"/>
-      <c r="X58" s="29"/>
-      <c r="Y58" s="29"/>
-      <c r="Z58" s="29"/>
-      <c r="AA58" s="29"/>
-      <c r="AB58" s="29"/>
-      <c r="AC58" s="29"/>
-      <c r="AD58" s="29"/>
-      <c r="AE58" s="29"/>
-      <c r="AF58" s="29"/>
-      <c r="AG58" s="29"/>
-      <c r="AH58" s="29"/>
-      <c r="AI58" s="29"/>
-      <c r="AJ58" s="29"/>
-      <c r="AK58" s="29"/>
-      <c r="AL58" s="29"/>
-      <c r="AM58" s="29"/>
-      <c r="AN58" s="29"/>
-      <c r="AO58" s="29"/>
-      <c r="AP58" s="29"/>
-      <c r="AQ58" s="29"/>
-      <c r="AR58" s="29"/>
-      <c r="AS58" s="29"/>
-      <c r="AT58" s="29"/>
-      <c r="AU58" s="29"/>
-    </row>
-    <row r="59" spans="1:47">
-      <c r="A59" s="29"/>
-      <c r="B59" s="29"/>
-      <c r="C59" s="29"/>
-      <c r="D59" s="29"/>
-      <c r="E59" s="29"/>
-      <c r="F59" s="29"/>
-      <c r="G59" s="29"/>
-      <c r="H59" s="29"/>
-      <c r="I59" s="29"/>
-      <c r="J59" s="29"/>
-      <c r="K59" s="29"/>
-      <c r="L59" s="29"/>
-      <c r="M59" s="29"/>
-      <c r="N59" s="29"/>
-      <c r="O59" s="29"/>
-      <c r="P59" s="29"/>
-      <c r="Q59" s="29"/>
-      <c r="R59" s="29"/>
-      <c r="S59" s="29"/>
-      <c r="T59" s="29"/>
-      <c r="U59" s="29"/>
-      <c r="V59" s="29"/>
-      <c r="W59" s="29"/>
-      <c r="X59" s="29"/>
-      <c r="Y59" s="29"/>
-      <c r="Z59" s="29"/>
-      <c r="AA59" s="29"/>
-      <c r="AB59" s="29"/>
-      <c r="AC59" s="29"/>
-      <c r="AD59" s="29"/>
-      <c r="AE59" s="29"/>
-      <c r="AF59" s="29"/>
-      <c r="AG59" s="29"/>
-      <c r="AH59" s="29"/>
-      <c r="AI59" s="29"/>
-      <c r="AJ59" s="29"/>
-      <c r="AK59" s="29"/>
-      <c r="AL59" s="29"/>
-      <c r="AM59" s="29"/>
-      <c r="AN59" s="29"/>
-      <c r="AO59" s="29"/>
-      <c r="AP59" s="29"/>
-      <c r="AQ59" s="29"/>
-      <c r="AR59" s="29"/>
-      <c r="AS59" s="29"/>
-      <c r="AT59" s="29"/>
-      <c r="AU59" s="29"/>
-    </row>
-    <row r="60" spans="1:47">
-      <c r="A60" s="29"/>
-      <c r="B60" s="29"/>
-      <c r="C60" s="29"/>
-      <c r="D60" s="29"/>
-      <c r="E60" s="29"/>
-      <c r="F60" s="29"/>
-      <c r="G60" s="29"/>
-      <c r="H60" s="29"/>
-      <c r="I60" s="29"/>
-      <c r="J60" s="29"/>
-      <c r="K60" s="29"/>
-      <c r="L60" s="29"/>
-      <c r="M60" s="29"/>
-      <c r="N60" s="29"/>
-      <c r="O60" s="29"/>
-      <c r="P60" s="29"/>
-      <c r="Q60" s="29"/>
-      <c r="R60" s="29"/>
-      <c r="S60" s="29"/>
-      <c r="T60" s="29"/>
-      <c r="U60" s="29"/>
-      <c r="V60" s="29"/>
-      <c r="W60" s="29"/>
-      <c r="X60" s="29"/>
-      <c r="Y60" s="29"/>
-      <c r="Z60" s="29"/>
-      <c r="AA60" s="29"/>
-      <c r="AB60" s="29"/>
-      <c r="AC60" s="29"/>
-      <c r="AD60" s="29"/>
-      <c r="AE60" s="29"/>
-      <c r="AF60" s="29"/>
-      <c r="AG60" s="29"/>
-      <c r="AH60" s="29"/>
-      <c r="AI60" s="29"/>
-      <c r="AJ60" s="29"/>
-      <c r="AK60" s="29"/>
-      <c r="AL60" s="29"/>
-      <c r="AM60" s="29"/>
-      <c r="AN60" s="29"/>
-      <c r="AO60" s="29"/>
-      <c r="AP60" s="29"/>
-      <c r="AQ60" s="29"/>
-      <c r="AR60" s="29"/>
-      <c r="AS60" s="29"/>
-      <c r="AT60" s="29"/>
-      <c r="AU60" s="29"/>
-    </row>
-    <row r="61" spans="1:47">
-      <c r="A61" s="29"/>
-      <c r="B61" s="29"/>
-      <c r="C61" s="29"/>
-      <c r="D61" s="29"/>
-      <c r="E61" s="29"/>
-      <c r="F61" s="29"/>
-      <c r="G61" s="29"/>
-      <c r="H61" s="29"/>
-      <c r="I61" s="29"/>
-      <c r="J61" s="29"/>
-      <c r="K61" s="29"/>
-      <c r="L61" s="29"/>
-      <c r="M61" s="29"/>
-      <c r="N61" s="29"/>
-      <c r="O61" s="29"/>
-      <c r="P61" s="29"/>
-      <c r="Q61" s="29"/>
-      <c r="R61" s="29"/>
-      <c r="S61" s="29"/>
-      <c r="T61" s="29"/>
-      <c r="U61" s="29"/>
-      <c r="V61" s="29"/>
-      <c r="W61" s="29"/>
-      <c r="X61" s="29"/>
-      <c r="Y61" s="29"/>
-      <c r="Z61" s="29"/>
-      <c r="AA61" s="29"/>
-      <c r="AB61" s="29"/>
-      <c r="AC61" s="29"/>
-      <c r="AD61" s="29"/>
-      <c r="AE61" s="29"/>
-      <c r="AF61" s="29"/>
-      <c r="AG61" s="29"/>
-      <c r="AH61" s="29"/>
-      <c r="AI61" s="29"/>
-      <c r="AJ61" s="29"/>
-      <c r="AK61" s="29"/>
-      <c r="AL61" s="29"/>
-      <c r="AM61" s="29"/>
-      <c r="AN61" s="29"/>
-      <c r="AO61" s="29"/>
-      <c r="AP61" s="29"/>
-      <c r="AQ61" s="29"/>
-      <c r="AR61" s="29"/>
-      <c r="AS61" s="29"/>
-      <c r="AT61" s="29"/>
-      <c r="AU61" s="29"/>
-    </row>
-    <row r="62" spans="1:47">
-      <c r="A62" s="29"/>
-      <c r="B62" s="29"/>
-      <c r="C62" s="29"/>
-      <c r="D62" s="29"/>
-      <c r="E62" s="29"/>
-      <c r="F62" s="29"/>
-      <c r="G62" s="29"/>
-      <c r="H62" s="29"/>
-      <c r="I62" s="29"/>
-      <c r="J62" s="29"/>
-      <c r="K62" s="29"/>
-      <c r="L62" s="29"/>
-      <c r="M62" s="29"/>
-      <c r="N62" s="29"/>
-      <c r="O62" s="29"/>
-      <c r="P62" s="29"/>
-      <c r="Q62" s="29"/>
-      <c r="R62" s="29"/>
-      <c r="S62" s="29"/>
-      <c r="T62" s="29"/>
-      <c r="U62" s="29"/>
-      <c r="V62" s="29"/>
-      <c r="W62" s="29"/>
-      <c r="X62" s="29"/>
-      <c r="Y62" s="29"/>
-      <c r="Z62" s="29"/>
-      <c r="AA62" s="29"/>
-      <c r="AB62" s="29"/>
-      <c r="AC62" s="29"/>
-      <c r="AD62" s="29"/>
-      <c r="AE62" s="29"/>
-      <c r="AF62" s="29"/>
-      <c r="AG62" s="29"/>
-      <c r="AH62" s="29"/>
-      <c r="AI62" s="29"/>
-      <c r="AJ62" s="29"/>
-      <c r="AK62" s="29"/>
-      <c r="AL62" s="29"/>
-      <c r="AM62" s="29"/>
-      <c r="AN62" s="29"/>
-      <c r="AO62" s="29"/>
-      <c r="AP62" s="29"/>
-      <c r="AQ62" s="29"/>
-      <c r="AR62" s="29"/>
-      <c r="AS62" s="29"/>
-      <c r="AT62" s="29"/>
-      <c r="AU62" s="29"/>
+    <row r="52" spans="1:47" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A52" s="72"/>
+      <c r="B52" s="68"/>
+      <c r="C52" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="D52" s="73"/>
+      <c r="E52" s="93"/>
+      <c r="F52" s="80"/>
+      <c r="G52" s="80"/>
+      <c r="H52" s="80"/>
+      <c r="I52" s="80"/>
+      <c r="J52" s="80"/>
+      <c r="K52" s="80"/>
+      <c r="L52" s="80"/>
+    </row>
+    <row r="53" spans="1:47" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A53" s="72"/>
+      <c r="B53" s="68"/>
+      <c r="C53" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="D53" s="73"/>
+      <c r="E53" s="93"/>
+      <c r="F53" s="80"/>
+      <c r="G53" s="80"/>
+      <c r="H53" s="80"/>
+      <c r="I53" s="80"/>
+      <c r="J53" s="80"/>
+      <c r="K53" s="80"/>
+      <c r="L53" s="80"/>
+    </row>
+    <row r="54" spans="1:47" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A54" s="72"/>
+      <c r="B54" s="68"/>
+      <c r="C54" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="D54" s="73"/>
+      <c r="E54" s="93"/>
+      <c r="F54" s="80"/>
+      <c r="G54" s="80"/>
+      <c r="H54" s="80"/>
+      <c r="I54" s="80"/>
+      <c r="J54" s="80"/>
+      <c r="K54" s="80"/>
+      <c r="L54" s="80"/>
+    </row>
+    <row r="55" spans="1:47" s="28" customFormat="1" ht="37.200000000000003" customHeight="1" outlineLevel="1">
+      <c r="A55" s="72"/>
+      <c r="B55" s="68"/>
+      <c r="C55" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="D55" s="73"/>
+      <c r="E55" s="93"/>
+      <c r="F55" s="80"/>
+      <c r="G55" s="80"/>
+      <c r="H55" s="80"/>
+      <c r="I55" s="80"/>
+      <c r="J55" s="80"/>
+      <c r="K55" s="80"/>
+      <c r="L55" s="80"/>
+    </row>
+    <row r="56" spans="1:47" s="12" customFormat="1" ht="13.2">
+      <c r="A56" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="B56" s="62" t="s">
+        <v>211</v>
+      </c>
+      <c r="C56" s="63"/>
+      <c r="D56" s="64"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="31"/>
+      <c r="G56" s="31"/>
+      <c r="H56" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="I56" s="33"/>
+      <c r="J56" s="33"/>
+      <c r="K56" s="33"/>
+      <c r="L56" s="33"/>
+    </row>
+    <row r="57" spans="1:47" s="28" customFormat="1" ht="44.4" customHeight="1" outlineLevel="1">
+      <c r="A57" s="72"/>
+      <c r="B57" s="68" t="s">
+        <v>164</v>
+      </c>
+      <c r="C57" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="D57" s="73" t="s">
+        <v>216</v>
+      </c>
+      <c r="E57" s="93"/>
+      <c r="F57" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="G57" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="H57" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="I57" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="J57" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="K57" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="L57" s="80" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:47" s="28" customFormat="1" ht="44.4" customHeight="1" outlineLevel="1">
+      <c r="A58" s="72"/>
+      <c r="B58" s="68"/>
+      <c r="C58" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="D58" s="73"/>
+      <c r="E58" s="93"/>
+      <c r="F58" s="80"/>
+      <c r="G58" s="80"/>
+      <c r="H58" s="80"/>
+      <c r="I58" s="80"/>
+      <c r="J58" s="80"/>
+      <c r="K58" s="80"/>
+      <c r="L58" s="80"/>
+    </row>
+    <row r="59" spans="1:47" s="28" customFormat="1" ht="44.4" customHeight="1" outlineLevel="1">
+      <c r="A59" s="72"/>
+      <c r="B59" s="68"/>
+      <c r="C59" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="D59" s="73"/>
+      <c r="E59" s="93"/>
+      <c r="F59" s="80"/>
+      <c r="G59" s="80"/>
+      <c r="H59" s="80"/>
+      <c r="I59" s="80"/>
+      <c r="J59" s="80"/>
+      <c r="K59" s="80"/>
+      <c r="L59" s="80"/>
+    </row>
+    <row r="60" spans="1:47" s="28" customFormat="1" ht="44.4" customHeight="1" outlineLevel="1">
+      <c r="A60" s="72"/>
+      <c r="B60" s="68"/>
+      <c r="C60" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="D60" s="73"/>
+      <c r="E60" s="93"/>
+      <c r="F60" s="80"/>
+      <c r="G60" s="80"/>
+      <c r="H60" s="80"/>
+      <c r="I60" s="80"/>
+      <c r="J60" s="80"/>
+      <c r="K60" s="80"/>
+      <c r="L60" s="80"/>
+    </row>
+    <row r="61" spans="1:47" s="28" customFormat="1" ht="44.4" customHeight="1" outlineLevel="1">
+      <c r="A61" s="72"/>
+      <c r="B61" s="68"/>
+      <c r="C61" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="D61" s="73"/>
+      <c r="E61" s="93"/>
+      <c r="F61" s="80"/>
+      <c r="G61" s="80"/>
+      <c r="H61" s="80"/>
+      <c r="I61" s="80"/>
+      <c r="J61" s="80"/>
+      <c r="K61" s="80"/>
+      <c r="L61" s="80"/>
+    </row>
+    <row r="62" spans="1:47" s="28" customFormat="1" ht="44.4" customHeight="1" outlineLevel="1">
+      <c r="A62" s="72"/>
+      <c r="B62" s="68"/>
+      <c r="C62" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="D62" s="73"/>
+      <c r="E62" s="93"/>
+      <c r="F62" s="80"/>
+      <c r="G62" s="80"/>
+      <c r="H62" s="80"/>
+      <c r="I62" s="80"/>
+      <c r="J62" s="80"/>
+      <c r="K62" s="80"/>
+      <c r="L62" s="80"/>
     </row>
     <row r="63" spans="1:47">
       <c r="A63" s="29"/>
@@ -50112,9 +49813,558 @@
       <c r="AT141" s="29"/>
       <c r="AU141" s="29"/>
     </row>
+    <row r="142" spans="1:47">
+      <c r="A142" s="29"/>
+      <c r="B142" s="29"/>
+      <c r="C142" s="29"/>
+      <c r="D142" s="29"/>
+      <c r="E142" s="29"/>
+      <c r="F142" s="29"/>
+      <c r="G142" s="29"/>
+      <c r="H142" s="29"/>
+      <c r="I142" s="29"/>
+      <c r="J142" s="29"/>
+      <c r="K142" s="29"/>
+      <c r="L142" s="29"/>
+      <c r="M142" s="29"/>
+      <c r="N142" s="29"/>
+      <c r="O142" s="29"/>
+      <c r="P142" s="29"/>
+      <c r="Q142" s="29"/>
+      <c r="R142" s="29"/>
+      <c r="S142" s="29"/>
+      <c r="T142" s="29"/>
+      <c r="U142" s="29"/>
+      <c r="V142" s="29"/>
+      <c r="W142" s="29"/>
+      <c r="X142" s="29"/>
+      <c r="Y142" s="29"/>
+      <c r="Z142" s="29"/>
+      <c r="AA142" s="29"/>
+      <c r="AB142" s="29"/>
+      <c r="AC142" s="29"/>
+      <c r="AD142" s="29"/>
+      <c r="AE142" s="29"/>
+      <c r="AF142" s="29"/>
+      <c r="AG142" s="29"/>
+      <c r="AH142" s="29"/>
+      <c r="AI142" s="29"/>
+      <c r="AJ142" s="29"/>
+      <c r="AK142" s="29"/>
+      <c r="AL142" s="29"/>
+      <c r="AM142" s="29"/>
+      <c r="AN142" s="29"/>
+      <c r="AO142" s="29"/>
+      <c r="AP142" s="29"/>
+      <c r="AQ142" s="29"/>
+      <c r="AR142" s="29"/>
+      <c r="AS142" s="29"/>
+      <c r="AT142" s="29"/>
+      <c r="AU142" s="29"/>
+    </row>
+    <row r="143" spans="1:47">
+      <c r="A143" s="29"/>
+      <c r="B143" s="29"/>
+      <c r="C143" s="29"/>
+      <c r="D143" s="29"/>
+      <c r="E143" s="29"/>
+      <c r="F143" s="29"/>
+      <c r="G143" s="29"/>
+      <c r="H143" s="29"/>
+      <c r="I143" s="29"/>
+      <c r="J143" s="29"/>
+      <c r="K143" s="29"/>
+      <c r="L143" s="29"/>
+      <c r="M143" s="29"/>
+      <c r="N143" s="29"/>
+      <c r="O143" s="29"/>
+      <c r="P143" s="29"/>
+      <c r="Q143" s="29"/>
+      <c r="R143" s="29"/>
+      <c r="S143" s="29"/>
+      <c r="T143" s="29"/>
+      <c r="U143" s="29"/>
+      <c r="V143" s="29"/>
+      <c r="W143" s="29"/>
+      <c r="X143" s="29"/>
+      <c r="Y143" s="29"/>
+      <c r="Z143" s="29"/>
+      <c r="AA143" s="29"/>
+      <c r="AB143" s="29"/>
+      <c r="AC143" s="29"/>
+      <c r="AD143" s="29"/>
+      <c r="AE143" s="29"/>
+      <c r="AF143" s="29"/>
+      <c r="AG143" s="29"/>
+      <c r="AH143" s="29"/>
+      <c r="AI143" s="29"/>
+      <c r="AJ143" s="29"/>
+      <c r="AK143" s="29"/>
+      <c r="AL143" s="29"/>
+      <c r="AM143" s="29"/>
+      <c r="AN143" s="29"/>
+      <c r="AO143" s="29"/>
+      <c r="AP143" s="29"/>
+      <c r="AQ143" s="29"/>
+      <c r="AR143" s="29"/>
+      <c r="AS143" s="29"/>
+      <c r="AT143" s="29"/>
+      <c r="AU143" s="29"/>
+    </row>
+    <row r="144" spans="1:47">
+      <c r="A144" s="29"/>
+      <c r="B144" s="29"/>
+      <c r="C144" s="29"/>
+      <c r="D144" s="29"/>
+      <c r="E144" s="29"/>
+      <c r="F144" s="29"/>
+      <c r="G144" s="29"/>
+      <c r="H144" s="29"/>
+      <c r="I144" s="29"/>
+      <c r="J144" s="29"/>
+      <c r="K144" s="29"/>
+      <c r="L144" s="29"/>
+      <c r="M144" s="29"/>
+      <c r="N144" s="29"/>
+      <c r="O144" s="29"/>
+      <c r="P144" s="29"/>
+      <c r="Q144" s="29"/>
+      <c r="R144" s="29"/>
+      <c r="S144" s="29"/>
+      <c r="T144" s="29"/>
+      <c r="U144" s="29"/>
+      <c r="V144" s="29"/>
+      <c r="W144" s="29"/>
+      <c r="X144" s="29"/>
+      <c r="Y144" s="29"/>
+      <c r="Z144" s="29"/>
+      <c r="AA144" s="29"/>
+      <c r="AB144" s="29"/>
+      <c r="AC144" s="29"/>
+      <c r="AD144" s="29"/>
+      <c r="AE144" s="29"/>
+      <c r="AF144" s="29"/>
+      <c r="AG144" s="29"/>
+      <c r="AH144" s="29"/>
+      <c r="AI144" s="29"/>
+      <c r="AJ144" s="29"/>
+      <c r="AK144" s="29"/>
+      <c r="AL144" s="29"/>
+      <c r="AM144" s="29"/>
+      <c r="AN144" s="29"/>
+      <c r="AO144" s="29"/>
+      <c r="AP144" s="29"/>
+      <c r="AQ144" s="29"/>
+      <c r="AR144" s="29"/>
+      <c r="AS144" s="29"/>
+      <c r="AT144" s="29"/>
+      <c r="AU144" s="29"/>
+    </row>
+    <row r="145" spans="1:47">
+      <c r="A145" s="29"/>
+      <c r="B145" s="29"/>
+      <c r="C145" s="29"/>
+      <c r="D145" s="29"/>
+      <c r="E145" s="29"/>
+      <c r="F145" s="29"/>
+      <c r="G145" s="29"/>
+      <c r="H145" s="29"/>
+      <c r="I145" s="29"/>
+      <c r="J145" s="29"/>
+      <c r="K145" s="29"/>
+      <c r="L145" s="29"/>
+      <c r="M145" s="29"/>
+      <c r="N145" s="29"/>
+      <c r="O145" s="29"/>
+      <c r="P145" s="29"/>
+      <c r="Q145" s="29"/>
+      <c r="R145" s="29"/>
+      <c r="S145" s="29"/>
+      <c r="T145" s="29"/>
+      <c r="U145" s="29"/>
+      <c r="V145" s="29"/>
+      <c r="W145" s="29"/>
+      <c r="X145" s="29"/>
+      <c r="Y145" s="29"/>
+      <c r="Z145" s="29"/>
+      <c r="AA145" s="29"/>
+      <c r="AB145" s="29"/>
+      <c r="AC145" s="29"/>
+      <c r="AD145" s="29"/>
+      <c r="AE145" s="29"/>
+      <c r="AF145" s="29"/>
+      <c r="AG145" s="29"/>
+      <c r="AH145" s="29"/>
+      <c r="AI145" s="29"/>
+      <c r="AJ145" s="29"/>
+      <c r="AK145" s="29"/>
+      <c r="AL145" s="29"/>
+      <c r="AM145" s="29"/>
+      <c r="AN145" s="29"/>
+      <c r="AO145" s="29"/>
+      <c r="AP145" s="29"/>
+      <c r="AQ145" s="29"/>
+      <c r="AR145" s="29"/>
+      <c r="AS145" s="29"/>
+      <c r="AT145" s="29"/>
+      <c r="AU145" s="29"/>
+    </row>
+    <row r="146" spans="1:47">
+      <c r="A146" s="29"/>
+      <c r="B146" s="29"/>
+      <c r="C146" s="29"/>
+      <c r="D146" s="29"/>
+      <c r="E146" s="29"/>
+      <c r="F146" s="29"/>
+      <c r="G146" s="29"/>
+      <c r="H146" s="29"/>
+      <c r="I146" s="29"/>
+      <c r="J146" s="29"/>
+      <c r="K146" s="29"/>
+      <c r="L146" s="29"/>
+      <c r="M146" s="29"/>
+      <c r="N146" s="29"/>
+      <c r="O146" s="29"/>
+      <c r="P146" s="29"/>
+      <c r="Q146" s="29"/>
+      <c r="R146" s="29"/>
+      <c r="S146" s="29"/>
+      <c r="T146" s="29"/>
+      <c r="U146" s="29"/>
+      <c r="V146" s="29"/>
+      <c r="W146" s="29"/>
+      <c r="X146" s="29"/>
+      <c r="Y146" s="29"/>
+      <c r="Z146" s="29"/>
+      <c r="AA146" s="29"/>
+      <c r="AB146" s="29"/>
+      <c r="AC146" s="29"/>
+      <c r="AD146" s="29"/>
+      <c r="AE146" s="29"/>
+      <c r="AF146" s="29"/>
+      <c r="AG146" s="29"/>
+      <c r="AH146" s="29"/>
+      <c r="AI146" s="29"/>
+      <c r="AJ146" s="29"/>
+      <c r="AK146" s="29"/>
+      <c r="AL146" s="29"/>
+      <c r="AM146" s="29"/>
+      <c r="AN146" s="29"/>
+      <c r="AO146" s="29"/>
+      <c r="AP146" s="29"/>
+      <c r="AQ146" s="29"/>
+      <c r="AR146" s="29"/>
+      <c r="AS146" s="29"/>
+      <c r="AT146" s="29"/>
+      <c r="AU146" s="29"/>
+    </row>
+    <row r="147" spans="1:47">
+      <c r="A147" s="29"/>
+      <c r="B147" s="29"/>
+      <c r="C147" s="29"/>
+      <c r="D147" s="29"/>
+      <c r="E147" s="29"/>
+      <c r="F147" s="29"/>
+      <c r="G147" s="29"/>
+      <c r="H147" s="29"/>
+      <c r="I147" s="29"/>
+      <c r="J147" s="29"/>
+      <c r="K147" s="29"/>
+      <c r="L147" s="29"/>
+      <c r="M147" s="29"/>
+      <c r="N147" s="29"/>
+      <c r="O147" s="29"/>
+      <c r="P147" s="29"/>
+      <c r="Q147" s="29"/>
+      <c r="R147" s="29"/>
+      <c r="S147" s="29"/>
+      <c r="T147" s="29"/>
+      <c r="U147" s="29"/>
+      <c r="V147" s="29"/>
+      <c r="W147" s="29"/>
+      <c r="X147" s="29"/>
+      <c r="Y147" s="29"/>
+      <c r="Z147" s="29"/>
+      <c r="AA147" s="29"/>
+      <c r="AB147" s="29"/>
+      <c r="AC147" s="29"/>
+      <c r="AD147" s="29"/>
+      <c r="AE147" s="29"/>
+      <c r="AF147" s="29"/>
+      <c r="AG147" s="29"/>
+      <c r="AH147" s="29"/>
+      <c r="AI147" s="29"/>
+      <c r="AJ147" s="29"/>
+      <c r="AK147" s="29"/>
+      <c r="AL147" s="29"/>
+      <c r="AM147" s="29"/>
+      <c r="AN147" s="29"/>
+      <c r="AO147" s="29"/>
+      <c r="AP147" s="29"/>
+      <c r="AQ147" s="29"/>
+      <c r="AR147" s="29"/>
+      <c r="AS147" s="29"/>
+      <c r="AT147" s="29"/>
+      <c r="AU147" s="29"/>
+    </row>
+    <row r="148" spans="1:47">
+      <c r="A148" s="29"/>
+      <c r="B148" s="29"/>
+      <c r="C148" s="29"/>
+      <c r="D148" s="29"/>
+      <c r="E148" s="29"/>
+      <c r="F148" s="29"/>
+      <c r="G148" s="29"/>
+      <c r="H148" s="29"/>
+      <c r="I148" s="29"/>
+      <c r="J148" s="29"/>
+      <c r="K148" s="29"/>
+      <c r="L148" s="29"/>
+      <c r="M148" s="29"/>
+      <c r="N148" s="29"/>
+      <c r="O148" s="29"/>
+      <c r="P148" s="29"/>
+      <c r="Q148" s="29"/>
+      <c r="R148" s="29"/>
+      <c r="S148" s="29"/>
+      <c r="T148" s="29"/>
+      <c r="U148" s="29"/>
+      <c r="V148" s="29"/>
+      <c r="W148" s="29"/>
+      <c r="X148" s="29"/>
+      <c r="Y148" s="29"/>
+      <c r="Z148" s="29"/>
+      <c r="AA148" s="29"/>
+      <c r="AB148" s="29"/>
+      <c r="AC148" s="29"/>
+      <c r="AD148" s="29"/>
+      <c r="AE148" s="29"/>
+      <c r="AF148" s="29"/>
+      <c r="AG148" s="29"/>
+      <c r="AH148" s="29"/>
+      <c r="AI148" s="29"/>
+      <c r="AJ148" s="29"/>
+      <c r="AK148" s="29"/>
+      <c r="AL148" s="29"/>
+      <c r="AM148" s="29"/>
+      <c r="AN148" s="29"/>
+      <c r="AO148" s="29"/>
+      <c r="AP148" s="29"/>
+      <c r="AQ148" s="29"/>
+      <c r="AR148" s="29"/>
+      <c r="AS148" s="29"/>
+      <c r="AT148" s="29"/>
+      <c r="AU148" s="29"/>
+    </row>
+    <row r="149" spans="1:47">
+      <c r="A149" s="29"/>
+      <c r="B149" s="29"/>
+      <c r="C149" s="29"/>
+      <c r="D149" s="29"/>
+      <c r="E149" s="29"/>
+      <c r="F149" s="29"/>
+      <c r="G149" s="29"/>
+      <c r="H149" s="29"/>
+      <c r="I149" s="29"/>
+      <c r="J149" s="29"/>
+      <c r="K149" s="29"/>
+      <c r="L149" s="29"/>
+      <c r="M149" s="29"/>
+      <c r="N149" s="29"/>
+      <c r="O149" s="29"/>
+      <c r="P149" s="29"/>
+      <c r="Q149" s="29"/>
+      <c r="R149" s="29"/>
+      <c r="S149" s="29"/>
+      <c r="T149" s="29"/>
+      <c r="U149" s="29"/>
+      <c r="V149" s="29"/>
+      <c r="W149" s="29"/>
+      <c r="X149" s="29"/>
+      <c r="Y149" s="29"/>
+      <c r="Z149" s="29"/>
+      <c r="AA149" s="29"/>
+      <c r="AB149" s="29"/>
+      <c r="AC149" s="29"/>
+      <c r="AD149" s="29"/>
+      <c r="AE149" s="29"/>
+      <c r="AF149" s="29"/>
+      <c r="AG149" s="29"/>
+      <c r="AH149" s="29"/>
+      <c r="AI149" s="29"/>
+      <c r="AJ149" s="29"/>
+      <c r="AK149" s="29"/>
+      <c r="AL149" s="29"/>
+      <c r="AM149" s="29"/>
+      <c r="AN149" s="29"/>
+      <c r="AO149" s="29"/>
+      <c r="AP149" s="29"/>
+      <c r="AQ149" s="29"/>
+      <c r="AR149" s="29"/>
+      <c r="AS149" s="29"/>
+      <c r="AT149" s="29"/>
+      <c r="AU149" s="29"/>
+    </row>
+    <row r="150" spans="1:47">
+      <c r="A150" s="29"/>
+      <c r="B150" s="29"/>
+      <c r="C150" s="29"/>
+      <c r="D150" s="29"/>
+      <c r="E150" s="29"/>
+      <c r="F150" s="29"/>
+      <c r="G150" s="29"/>
+      <c r="H150" s="29"/>
+      <c r="I150" s="29"/>
+      <c r="J150" s="29"/>
+      <c r="K150" s="29"/>
+      <c r="L150" s="29"/>
+      <c r="M150" s="29"/>
+      <c r="N150" s="29"/>
+      <c r="O150" s="29"/>
+      <c r="P150" s="29"/>
+      <c r="Q150" s="29"/>
+      <c r="R150" s="29"/>
+      <c r="S150" s="29"/>
+      <c r="T150" s="29"/>
+      <c r="U150" s="29"/>
+      <c r="V150" s="29"/>
+      <c r="W150" s="29"/>
+      <c r="X150" s="29"/>
+      <c r="Y150" s="29"/>
+      <c r="Z150" s="29"/>
+      <c r="AA150" s="29"/>
+      <c r="AB150" s="29"/>
+      <c r="AC150" s="29"/>
+      <c r="AD150" s="29"/>
+      <c r="AE150" s="29"/>
+      <c r="AF150" s="29"/>
+      <c r="AG150" s="29"/>
+      <c r="AH150" s="29"/>
+      <c r="AI150" s="29"/>
+      <c r="AJ150" s="29"/>
+      <c r="AK150" s="29"/>
+      <c r="AL150" s="29"/>
+      <c r="AM150" s="29"/>
+      <c r="AN150" s="29"/>
+      <c r="AO150" s="29"/>
+      <c r="AP150" s="29"/>
+      <c r="AQ150" s="29"/>
+      <c r="AR150" s="29"/>
+      <c r="AS150" s="29"/>
+      <c r="AT150" s="29"/>
+      <c r="AU150" s="29"/>
+    </row>
+    <row r="151" spans="1:47">
+      <c r="A151" s="29"/>
+      <c r="B151" s="29"/>
+      <c r="C151" s="29"/>
+      <c r="D151" s="29"/>
+      <c r="E151" s="29"/>
+      <c r="F151" s="29"/>
+      <c r="G151" s="29"/>
+      <c r="H151" s="29"/>
+      <c r="I151" s="29"/>
+      <c r="J151" s="29"/>
+      <c r="K151" s="29"/>
+      <c r="L151" s="29"/>
+      <c r="M151" s="29"/>
+      <c r="N151" s="29"/>
+      <c r="O151" s="29"/>
+      <c r="P151" s="29"/>
+      <c r="Q151" s="29"/>
+      <c r="R151" s="29"/>
+      <c r="S151" s="29"/>
+      <c r="T151" s="29"/>
+      <c r="U151" s="29"/>
+      <c r="V151" s="29"/>
+      <c r="W151" s="29"/>
+      <c r="X151" s="29"/>
+      <c r="Y151" s="29"/>
+      <c r="Z151" s="29"/>
+      <c r="AA151" s="29"/>
+      <c r="AB151" s="29"/>
+      <c r="AC151" s="29"/>
+      <c r="AD151" s="29"/>
+      <c r="AE151" s="29"/>
+      <c r="AF151" s="29"/>
+      <c r="AG151" s="29"/>
+      <c r="AH151" s="29"/>
+      <c r="AI151" s="29"/>
+      <c r="AJ151" s="29"/>
+      <c r="AK151" s="29"/>
+      <c r="AL151" s="29"/>
+      <c r="AM151" s="29"/>
+      <c r="AN151" s="29"/>
+      <c r="AO151" s="29"/>
+      <c r="AP151" s="29"/>
+      <c r="AQ151" s="29"/>
+      <c r="AR151" s="29"/>
+      <c r="AS151" s="29"/>
+      <c r="AT151" s="29"/>
+      <c r="AU151" s="29"/>
+    </row>
+    <row r="152" spans="1:47">
+      <c r="A152" s="29"/>
+      <c r="B152" s="29"/>
+      <c r="C152" s="29"/>
+      <c r="D152" s="29"/>
+      <c r="E152" s="29"/>
+      <c r="F152" s="29"/>
+      <c r="G152" s="29"/>
+      <c r="H152" s="29"/>
+      <c r="I152" s="29"/>
+      <c r="J152" s="29"/>
+      <c r="K152" s="29"/>
+      <c r="L152" s="29"/>
+      <c r="M152" s="29"/>
+      <c r="N152" s="29"/>
+      <c r="O152" s="29"/>
+      <c r="P152" s="29"/>
+      <c r="Q152" s="29"/>
+      <c r="R152" s="29"/>
+      <c r="S152" s="29"/>
+      <c r="T152" s="29"/>
+      <c r="U152" s="29"/>
+      <c r="V152" s="29"/>
+      <c r="W152" s="29"/>
+      <c r="X152" s="29"/>
+      <c r="Y152" s="29"/>
+      <c r="Z152" s="29"/>
+      <c r="AA152" s="29"/>
+      <c r="AB152" s="29"/>
+      <c r="AC152" s="29"/>
+      <c r="AD152" s="29"/>
+      <c r="AE152" s="29"/>
+      <c r="AF152" s="29"/>
+      <c r="AG152" s="29"/>
+      <c r="AH152" s="29"/>
+      <c r="AI152" s="29"/>
+      <c r="AJ152" s="29"/>
+      <c r="AK152" s="29"/>
+      <c r="AL152" s="29"/>
+      <c r="AM152" s="29"/>
+      <c r="AN152" s="29"/>
+      <c r="AO152" s="29"/>
+      <c r="AP152" s="29"/>
+      <c r="AQ152" s="29"/>
+      <c r="AR152" s="29"/>
+      <c r="AS152" s="29"/>
+      <c r="AT152" s="29"/>
+      <c r="AU152" s="29"/>
+    </row>
   </sheetData>
   <autoFilter ref="A22:L22" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
-  <mergeCells count="59">
+  <mergeCells count="71">
+    <mergeCell ref="H40:H45"/>
+    <mergeCell ref="I40:I45"/>
+    <mergeCell ref="J40:J45"/>
+    <mergeCell ref="K40:K45"/>
+    <mergeCell ref="L40:L45"/>
+    <mergeCell ref="B40:B45"/>
+    <mergeCell ref="D40:D45"/>
+    <mergeCell ref="E40:E45"/>
+    <mergeCell ref="F40:F45"/>
+    <mergeCell ref="G40:G45"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:C3"/>
@@ -50128,16 +50378,16 @@
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="H21:L21"/>
     <mergeCell ref="L24:L28"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="D30:D34"/>
-    <mergeCell ref="F30:F34"/>
-    <mergeCell ref="G30:G34"/>
-    <mergeCell ref="H30:H34"/>
-    <mergeCell ref="I30:I34"/>
-    <mergeCell ref="J30:J34"/>
+    <mergeCell ref="A30:A38"/>
+    <mergeCell ref="B30:B38"/>
+    <mergeCell ref="D30:D38"/>
+    <mergeCell ref="F30:F38"/>
+    <mergeCell ref="G30:G38"/>
+    <mergeCell ref="H30:H38"/>
+    <mergeCell ref="I30:I38"/>
+    <mergeCell ref="J30:J38"/>
     <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E30:E34"/>
+    <mergeCell ref="E30:E38"/>
     <mergeCell ref="G24:G28"/>
     <mergeCell ref="H24:H28"/>
     <mergeCell ref="I24:I28"/>
@@ -50148,49 +50398,51 @@
     <mergeCell ref="D24:D28"/>
     <mergeCell ref="E24:E28"/>
     <mergeCell ref="F24:F28"/>
-    <mergeCell ref="K30:K34"/>
-    <mergeCell ref="L30:L34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="A36:A44"/>
-    <mergeCell ref="B36:B44"/>
-    <mergeCell ref="D36:D44"/>
-    <mergeCell ref="E36:E44"/>
-    <mergeCell ref="F36:F44"/>
-    <mergeCell ref="G36:G44"/>
-    <mergeCell ref="H36:H44"/>
-    <mergeCell ref="I36:I44"/>
-    <mergeCell ref="J36:J44"/>
-    <mergeCell ref="K36:K44"/>
-    <mergeCell ref="L36:L44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="A46:A51"/>
-    <mergeCell ref="B46:B51"/>
-    <mergeCell ref="D46:D51"/>
-    <mergeCell ref="E46:E51"/>
-    <mergeCell ref="K46:K51"/>
-    <mergeCell ref="L46:L51"/>
-    <mergeCell ref="F46:F51"/>
-    <mergeCell ref="G46:G51"/>
-    <mergeCell ref="H46:H51"/>
-    <mergeCell ref="I46:I51"/>
-    <mergeCell ref="J46:J51"/>
+    <mergeCell ref="K30:K38"/>
+    <mergeCell ref="L30:L38"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="A47:A55"/>
+    <mergeCell ref="B47:B55"/>
+    <mergeCell ref="D47:D55"/>
+    <mergeCell ref="E47:E55"/>
+    <mergeCell ref="F47:F55"/>
+    <mergeCell ref="G47:G55"/>
+    <mergeCell ref="H47:H55"/>
+    <mergeCell ref="I47:I55"/>
+    <mergeCell ref="J47:J55"/>
+    <mergeCell ref="K47:K55"/>
+    <mergeCell ref="L47:L55"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="A40:A45"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="A57:A62"/>
+    <mergeCell ref="B57:B62"/>
+    <mergeCell ref="D57:D62"/>
+    <mergeCell ref="E57:E62"/>
+    <mergeCell ref="K57:K62"/>
+    <mergeCell ref="L57:L62"/>
+    <mergeCell ref="F57:F62"/>
+    <mergeCell ref="G57:G62"/>
+    <mergeCell ref="H57:H62"/>
+    <mergeCell ref="I57:I62"/>
+    <mergeCell ref="J57:J62"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" sqref="MFX23:MGA51 AMR23:AMU51 SHL23:SHO51 AWN23:AWQ51 MPT23:MPW51 BGJ23:BGM51 VIF23:VII51 BQF23:BQI51 MZP23:MZS51 CAB23:CAE51 SRH23:SRK51 CJX23:CKA51 NJL23:NJO51 CTT23:CTW51 WVP23:WVS51 DDP23:DDS51 NTH23:NTK51 DNL23:DNO51 TBD23:TBG51 DXH23:DXK51 ODD23:ODG51 EHD23:EHG51 VSB23:VSE51 EQZ23:ERC51 OMZ23:ONC51 FAV23:FAY51 TKZ23:TLC51 FKR23:FKU51 OWV23:OWY51 FUN23:FUQ51 JD23:JG51 GEJ23:GEM51 PGR23:PGU51 GOF23:GOI51 TUV23:TUY51 GYB23:GYE51 PQN23:PQQ51 HHX23:HIA51 WBX23:WCA51 HRT23:HRW51 QAJ23:QAM51 IBP23:IBS51 UER23:UEU51 ILL23:ILO51 QKF23:QKI51 IVH23:IVK51 SZ23:TC51 JFD23:JFG51 QUB23:QUE51 JOZ23:JPC51 UON23:UOQ51 JYV23:JYY51 RDX23:REA51 KIR23:KIU51 WLT23:WLW51 KSN23:KSQ51 RNT23:RNW51 LCJ23:LCM51 UYJ23:UYM51 LMF23:LMI51 RXP23:RXS51 LWB23:LWE51 ACV23:ACY51" xr:uid="{F10FE83F-61D8-4140-B18D-7D0CA26FA4EB}">
-      <formula1>$A$14:$A$19</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="H23:L23 H29:L29 H35:L35 H45:L45" xr:uid="{4E16EDCF-1303-49A3-B4E2-32D5BBAC46DF}">
+    <dataValidation type="list" allowBlank="1" sqref="H23:L23 H29:L29 H46:L46 H56:L56 H39:L39" xr:uid="{4E16EDCF-1303-49A3-B4E2-32D5BBAC46DF}">
       <formula1>$B$13:$G$13</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{52397D1C-D727-4879-8F3C-C418CCE9A0FD}">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation showDropDown="1" showErrorMessage="1" sqref="JE21:JG22 TA21:TC22 ACW21:ACY22 AMS21:AMU22 AWO21:AWQ22 BGK21:BGM22 BQG21:BQI22 CAC21:CAE22 CJY21:CKA22 CTU21:CTW22 DDQ21:DDS22 DNM21:DNO22 DXI21:DXK22 EHE21:EHG22 ERA21:ERC22 FAW21:FAY22 FKS21:FKU22 FUO21:FUQ22 GEK21:GEM22 GOG21:GOI22 GYC21:GYE22 HHY21:HIA22 HRU21:HRW22 IBQ21:IBS22 ILM21:ILO22 IVI21:IVK22 JFE21:JFG22 JPA21:JPC22 JYW21:JYY22 KIS21:KIU22 KSO21:KSQ22 LCK21:LCM22 LMG21:LMI22 LWC21:LWE22 MFY21:MGA22 MPU21:MPW22 MZQ21:MZS22 NJM21:NJO22 NTI21:NTK22 ODE21:ODG22 ONA21:ONC22 OWW21:OWY22 PGS21:PGU22 PQO21:PQQ22 QAK21:QAM22 QKG21:QKI22 QUC21:QUE22 RDY21:REA22 RNU21:RNW22 RXQ21:RXS22 SHM21:SHO22 SRI21:SRK22 TBE21:TBG22 TLA21:TLC22 TUW21:TUY22 UES21:UEU22 UOO21:UOQ22 UYK21:UYM22 VIG21:VII22 VSC21:VSE22 WBY21:WCA22 WLU21:WLW22 WVQ21:WVS22 H21 H22:L22" xr:uid="{D568824C-3C41-440E-8D35-AA20C3943BBD}"/>
+    <dataValidation type="list" allowBlank="1" sqref="ACV23:ACY62 LWB23:LWE62 RXP23:RXS62 LMF23:LMI62 UYJ23:UYM62 LCJ23:LCM62 RNT23:RNW62 KSN23:KSQ62 WLT23:WLW62 KIR23:KIU62 RDX23:REA62 JYV23:JYY62 UON23:UOQ62 JOZ23:JPC62 QUB23:QUE62 JFD23:JFG62 SZ23:TC62 IVH23:IVK62 QKF23:QKI62 ILL23:ILO62 UER23:UEU62 IBP23:IBS62 QAJ23:QAM62 HRT23:HRW62 WBX23:WCA62 HHX23:HIA62 PQN23:PQQ62 GYB23:GYE62 TUV23:TUY62 GOF23:GOI62 PGR23:PGU62 GEJ23:GEM62 JD23:JG62 FUN23:FUQ62 OWV23:OWY62 FKR23:FKU62 TKZ23:TLC62 FAV23:FAY62 OMZ23:ONC62 EQZ23:ERC62 VSB23:VSE62 EHD23:EHG62 ODD23:ODG62 DXH23:DXK62 TBD23:TBG62 DNL23:DNO62 NTH23:NTK62 DDP23:DDS62 WVP23:WVS62 CTT23:CTW62 NJL23:NJO62 CJX23:CKA62 SRH23:SRK62 CAB23:CAE62 MZP23:MZS62 BQF23:BQI62 VIF23:VII62 BGJ23:BGM62 MPT23:MPW62 AWN23:AWQ62 SHL23:SHO62 AMR23:AMU62 MFX23:MGA62" xr:uid="{F10FE83F-61D8-4140-B18D-7D0CA26FA4EB}">
+      <formula1>$A$14:$A$19</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A23 A29 A35 A45" numberStoredAsText="1"/>
+    <ignoredError sqref="A23 A29 A39 A46 A56" numberStoredAsText="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>